<commit_message>
v of ganapati added
</commit_message>
<xml_diff>
--- a/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
+++ b/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate (3)" sheetId="19" r:id="rId1"/>
@@ -41,12 +41,12 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Estimate (3)'!$A$1:$K$90</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$99</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Estimate (3)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="82">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -419,16 +419,19 @@
   </si>
   <si>
     <t>-for steps</t>
+  </si>
+  <si>
+    <t>-partition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -632,7 +635,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -642,7 +645,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,14 +665,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,7 +681,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,7 +706,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,7 +736,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,7 +745,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -757,7 +760,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -773,11 +776,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,28 +795,51 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,9 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -840,41 +863,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1497,133 +1500,133 @@
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
       <c r="O6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="str">
         <f>B31</f>
@@ -1720,7 +1723,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -1752,7 +1755,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -1777,7 +1780,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -1797,7 +1800,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1821,7 +1824,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>64</v>
@@ -1848,7 +1851,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37"/>
       <c r="C16" s="19">
@@ -1873,7 +1876,7 @@
       <c r="J16" s="41"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37" t="s">
         <v>42</v>
@@ -1898,7 +1901,7 @@
       </c>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="37"/>
       <c r="C18" s="19"/>
@@ -1911,7 +1914,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:21" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>3</v>
       </c>
@@ -1928,7 +1931,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37" t="s">
         <v>66</v>
@@ -1954,7 +1957,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="37"/>
       <c r="C21" s="19">
@@ -1977,7 +1980,7 @@
       <c r="J21" s="41"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="37" t="s">
         <v>42</v>
@@ -2002,7 +2005,7 @@
       </c>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="37"/>
       <c r="C23" s="19"/>
@@ -2015,7 +2018,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>4</v>
       </c>
@@ -2032,7 +2035,7 @@
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="str">
         <f>B15</f>
@@ -2060,7 +2063,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37"/>
       <c r="C26" s="19">
@@ -2085,7 +2088,7 @@
       <c r="J26" s="41"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="37" t="s">
         <v>42</v>
@@ -2110,7 +2113,7 @@
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="37" t="s">
         <v>40</v>
@@ -2128,7 +2131,7 @@
       </c>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="37"/>
       <c r="C29" s="19"/>
@@ -2141,7 +2144,7 @@
       <c r="J29" s="41"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>5</v>
       </c>
@@ -2159,17 +2162,17 @@
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="85" t="s">
+      <c r="O30" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="85"/>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="85"/>
-      <c r="S30" s="85"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="85"/>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P30" s="81"/>
+      <c r="Q30" s="81"/>
+      <c r="R30" s="81"/>
+      <c r="S30" s="81"/>
+      <c r="T30" s="81"/>
+      <c r="U30" s="81"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37" t="str">
         <f>B36</f>
@@ -2205,7 +2208,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
         <v>42</v>
@@ -2230,7 +2233,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>40</v>
@@ -2248,7 +2251,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37"/>
       <c r="C34" s="42"/>
@@ -2261,7 +2264,7 @@
       <c r="J34" s="45"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <v>6</v>
       </c>
@@ -2285,7 +2288,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="37" t="s">
         <v>62</v>
@@ -2320,7 +2323,7 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="37"/>
       <c r="C37" s="36">
@@ -2352,7 +2355,7 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="37" t="str">
         <f>B25</f>
@@ -2389,7 +2392,7 @@
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="37"/>
       <c r="C39" s="47">
@@ -2423,7 +2426,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="37" t="s">
         <v>73</v>
@@ -2457,7 +2460,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="37"/>
       <c r="C41" s="47">
@@ -2489,7 +2492,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="37" t="s">
         <v>42</v>
@@ -2514,7 +2517,7 @@
       </c>
       <c r="K42" s="36"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="37" t="s">
         <v>40</v>
@@ -2532,7 +2535,7 @@
       </c>
       <c r="K43" s="36"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="37"/>
       <c r="C44" s="42"/>
@@ -2545,7 +2548,7 @@
       <c r="J44" s="45"/>
       <c r="K44" s="36"/>
     </row>
-    <row r="45" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A45" s="63">
         <v>7</v>
       </c>
@@ -2562,7 +2565,7 @@
       <c r="J45" s="45"/>
       <c r="K45" s="29"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>62</v>
@@ -2597,7 +2600,7 @@
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="37" t="s">
         <v>42</v>
@@ -2622,7 +2625,7 @@
       </c>
       <c r="K47" s="36"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="37" t="s">
         <v>40</v>
@@ -2640,7 +2643,7 @@
       </c>
       <c r="K48" s="36"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="37"/>
       <c r="C49" s="42"/>
@@ -2653,7 +2656,7 @@
       <c r="J49" s="44"/>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
         <v>8</v>
       </c>
@@ -2670,7 +2673,7 @@
       <c r="J50" s="41"/>
       <c r="K50" s="21"/>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="B51" s="37" t="s">
         <v>56</v>
@@ -2696,7 +2699,7 @@
       <c r="J51" s="40"/>
       <c r="K51" s="21"/>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="37"/>
       <c r="C52" s="36">
@@ -2720,7 +2723,7 @@
       <c r="J52" s="40"/>
       <c r="K52" s="21"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="37" t="s">
         <v>59</v>
@@ -2746,7 +2749,7 @@
       <c r="J53" s="40"/>
       <c r="K53" s="21"/>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="37"/>
       <c r="C54" s="36">
@@ -2770,7 +2773,7 @@
       <c r="J54" s="40"/>
       <c r="K54" s="21"/>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
       <c r="B55" s="37" t="s">
         <v>60</v>
@@ -2796,7 +2799,7 @@
       <c r="J55" s="40"/>
       <c r="K55" s="21"/>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="B56" s="37" t="s">
         <v>76</v>
@@ -2816,7 +2819,7 @@
       <c r="J56" s="40"/>
       <c r="K56" s="21"/>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="37" t="s">
         <v>42</v>
@@ -2841,7 +2844,7 @@
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
       <c r="B58" s="37" t="s">
         <v>40</v>
@@ -2859,7 +2862,7 @@
       </c>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="37"/>
       <c r="C59" s="19"/>
@@ -2872,7 +2875,7 @@
       <c r="J59" s="41"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.3">
       <c r="A60" s="18">
         <v>9</v>
       </c>
@@ -2893,7 +2896,7 @@
         <v>37.665999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="37" t="str">
         <f>B38</f>
@@ -2934,7 +2937,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="37"/>
       <c r="C62" s="47">
@@ -2961,7 +2964,7 @@
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="37"/>
       <c r="C63" s="47">
@@ -2987,7 +2990,7 @@
       <c r="J63" s="40"/>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="37"/>
       <c r="C64" s="47">
@@ -3014,7 +3017,7 @@
       <c r="J64" s="40"/>
       <c r="K64" s="21"/>
     </row>
-    <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="37" t="s">
         <v>75</v>
@@ -3040,7 +3043,7 @@
       <c r="J65" s="40"/>
       <c r="K65" s="21"/>
     </row>
-    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="37" t="s">
         <v>42</v>
@@ -3065,7 +3068,7 @@
       </c>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
       <c r="B67" s="37" t="s">
         <v>40</v>
@@ -3087,7 +3090,7 @@
         <v>4.2669917708015843</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="37"/>
       <c r="C68" s="19"/>
@@ -3100,7 +3103,7 @@
       <c r="J68" s="41"/>
       <c r="K68" s="21"/>
     </row>
-    <row r="69" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A69" s="18">
         <v>10</v>
       </c>
@@ -3127,7 +3130,7 @@
       <c r="J69" s="41"/>
       <c r="K69" s="21"/>
     </row>
-    <row r="70" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="B70" s="37" t="s">
         <v>71</v>
@@ -3156,7 +3159,7 @@
       <c r="J70" s="41"/>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="37" t="s">
         <v>72</v>
@@ -3186,7 +3189,7 @@
       <c r="J71" s="41"/>
       <c r="K71" s="21"/>
     </row>
-    <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="37" t="s">
         <v>42</v>
@@ -3211,7 +3214,7 @@
       </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="37" t="s">
         <v>40</v>
@@ -3229,7 +3232,7 @@
       </c>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="37"/>
       <c r="C74" s="19"/>
@@ -3242,7 +3245,7 @@
       <c r="J74" s="41"/>
       <c r="K74" s="21"/>
     </row>
-    <row r="75" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>11</v>
       </c>
@@ -3259,7 +3262,7 @@
       <c r="J75" s="41"/>
       <c r="K75" s="21"/>
     </row>
-    <row r="76" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18"/>
       <c r="B76" s="37" t="s">
         <v>56</v>
@@ -3284,7 +3287,7 @@
       <c r="J76" s="40"/>
       <c r="K76" s="21"/>
     </row>
-    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18"/>
       <c r="B77" s="37"/>
       <c r="C77" s="36">
@@ -3307,7 +3310,7 @@
       <c r="J77" s="40"/>
       <c r="K77" s="21"/>
     </row>
-    <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="37" t="s">
         <v>42</v>
@@ -3332,7 +3335,7 @@
       </c>
       <c r="K78" s="21"/>
     </row>
-    <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="37" t="s">
         <v>40</v>
@@ -3350,7 +3353,7 @@
       </c>
       <c r="K79" s="21"/>
     </row>
-    <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
       <c r="B80" s="37"/>
       <c r="C80" s="19"/>
@@ -3363,7 +3366,7 @@
       <c r="J80" s="41"/>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>12</v>
       </c>
@@ -3399,7 +3402,7 @@
       <c r="R81" s="25"/>
       <c r="S81" s="25"/>
     </row>
-    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18"/>
       <c r="B82" s="24"/>
       <c r="C82" s="19"/>
@@ -3422,7 +3425,7 @@
       <c r="R82" s="25"/>
       <c r="S82" s="25"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="46" t="s">
         <v>17</v>
@@ -3440,7 +3443,7 @@
       </c>
       <c r="K83" s="36"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="58"/>
       <c r="B84" s="61"/>
       <c r="C84" s="62"/>
@@ -3453,16 +3456,16 @@
       <c r="J84" s="60"/>
       <c r="K84" s="57"/>
     </row>
-    <row r="85" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="50"/>
       <c r="B85" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C85" s="90">
+      <c r="C85" s="77">
         <f>J83</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D85" s="90"/>
+      <c r="D85" s="77"/>
       <c r="E85" s="39">
         <v>100</v>
       </c>
@@ -3473,15 +3476,15 @@
       <c r="J85" s="54"/>
       <c r="K85" s="55"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="56"/>
       <c r="B86" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="93">
+      <c r="C86" s="80">
         <v>500000</v>
       </c>
-      <c r="D86" s="93"/>
+      <c r="D86" s="80"/>
       <c r="E86" s="39"/>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -3490,16 +3493,16 @@
       <c r="J86" s="48"/>
       <c r="K86" s="49"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="56"/>
       <c r="B87" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="93">
+      <c r="C87" s="80">
         <f>C86-C89-C90</f>
         <v>475000</v>
       </c>
-      <c r="D87" s="93"/>
+      <c r="D87" s="80"/>
       <c r="E87" s="39">
         <f>C87/C85*100</f>
         <v>84.274408192973809</v>
@@ -3511,16 +3514,16 @@
       <c r="J87" s="48"/>
       <c r="K87" s="49"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="56"/>
       <c r="B88" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C88" s="90">
+      <c r="C88" s="77">
         <f>C85-C87</f>
         <v>88634.928070135182</v>
       </c>
-      <c r="D88" s="90"/>
+      <c r="D88" s="77"/>
       <c r="E88" s="39">
         <f>100-E87</f>
         <v>15.725591807026191</v>
@@ -3532,16 +3535,16 @@
       <c r="J88" s="48"/>
       <c r="K88" s="49"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="56"/>
       <c r="B89" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="90">
+      <c r="C89" s="77">
         <f>C86*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D89" s="90"/>
+      <c r="D89" s="77"/>
       <c r="E89" s="39">
         <v>3</v>
       </c>
@@ -3552,16 +3555,16 @@
       <c r="J89" s="48"/>
       <c r="K89" s="49"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="56"/>
       <c r="B90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="90">
+      <c r="C90" s="77">
         <f>C86*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D90" s="90"/>
+      <c r="D90" s="77"/>
       <c r="E90" s="39">
         <v>2</v>
       </c>
@@ -3572,7 +3575,7 @@
       <c r="J90" s="48"/>
       <c r="K90" s="49"/>
     </row>
-    <row r="91" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="57"/>
       <c r="B91" s="57"/>
       <c r="C91" s="57"/>
@@ -3585,64 +3588,72 @@
       <c r="J91" s="57"/>
       <c r="K91" s="57"/>
     </row>
-    <row r="92" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O30:U30"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="A7:F7"/>
@@ -3651,14 +3662,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="O30:U30"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -3673,110 +3676,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-    </row>
-    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="74" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+    </row>
+    <row r="2" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="71">
+      <c r="C6" s="95">
         <f>F46</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3784,90 +3787,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="71">
+      <c r="J6" s="95">
         <f>I46</f>
-        <v>565521.79621734493</v>
-      </c>
-      <c r="K6" s="72"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>570675.01263534476</v>
+      </c>
+      <c r="K6" s="96"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="I7" s="81" t="s">
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="I7" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="e">
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="82" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="I8" s="82" t="s">
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="I8" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="e">
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="93" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="I9" s="82" t="s">
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="I9" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84" t="s">
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="77" t="s">
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="78" t="s">
+      <c r="K11" s="89" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3886,10 +3889,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="77"/>
-      <c r="K12" s="78"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="88"/>
+      <c r="K12" s="89"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <f>'Estimate (3)'!A9</f>
         <v>1</v>
@@ -3936,7 +3939,7 @@
         <v>1429.93875</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="32" t="str">
         <f>'Estimate (3)'!B12</f>
@@ -3965,7 +3968,7 @@
         <v>154.07112500000005</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -3982,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>'Estimate (3)'!A14</f>
         <v>2</v>
@@ -4029,7 +4032,7 @@
         <v>4355.6253171670223</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -4039,14 +4042,17 @@
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
-      <c r="J17" s="28"/>
+      <c r="J17" s="28">
+        <f>I17-F17</f>
+        <v>0</v>
+      </c>
       <c r="K17" s="14"/>
       <c r="M17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <f>'Estimate (3)'!A19</f>
         <v>3</v>
@@ -4093,7 +4099,7 @@
         <v>195.49218378543131</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="12"/>
@@ -4110,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f>'Estimate (3)'!A24</f>
         <v>4</v>
@@ -4157,7 +4163,7 @@
         <v>8886.4010857970134</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="32" t="str">
         <f>'Estimate (3)'!B28</f>
@@ -4176,14 +4182,17 @@
         <f>V!J27</f>
         <v>1052.5478821812251</v>
       </c>
-      <c r="J21" s="28"/>
+      <c r="J21" s="28">
+        <f>I21-F21</f>
+        <v>267.90467840188933</v>
+      </c>
       <c r="K21" s="14"/>
       <c r="M21" s="1">
         <f t="shared" si="0"/>
         <v>980.80400472416966</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="12"/>
@@ -4200,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <f>'Estimate (3)'!A30</f>
         <v>5</v>
@@ -4247,7 +4256,7 @@
         <v>14717.063250000003</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="32" t="str">
         <f>'Estimate (3)'!B33</f>
@@ -4266,14 +4275,17 @@
         <f>V!J34</f>
         <v>1177.0968081599999</v>
       </c>
-      <c r="J24" s="28"/>
+      <c r="J24" s="28">
+        <f>I24-F24</f>
+        <v>154.23788015999969</v>
+      </c>
       <c r="K24" s="14"/>
       <c r="M24" s="1">
         <f t="shared" si="0"/>
         <v>1278.5736600000002</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="12"/>
@@ -4290,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <f>'Estimate (3)'!A35</f>
         <v>6</v>
@@ -4337,7 +4349,7 @@
         <v>37921.213820481564</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
       <c r="B27" s="32" t="str">
         <f>'Estimate (3)'!B43</f>
@@ -4356,14 +4368,17 @@
         <f>V!J49</f>
         <v>2733.3234414988206</v>
       </c>
-      <c r="J27" s="28"/>
+      <c r="J27" s="28">
+        <f>I27-F27</f>
+        <v>-259.25455691922298</v>
+      </c>
       <c r="K27" s="14"/>
       <c r="M27" s="1">
         <f t="shared" si="0"/>
         <v>3740.7224980225546</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="12"/>
@@ -4380,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <f>'Estimate (3)'!A45</f>
         <v>7</v>
@@ -4427,7 +4442,7 @@
         <v>418901.22056250001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="32" t="str">
         <f>'Estimate (3)'!B48</f>
@@ -4446,14 +4461,17 @@
         <f>V!J56</f>
         <v>24340.57024335301</v>
       </c>
-      <c r="J30" s="28"/>
+      <c r="J30" s="28">
+        <f>I30-F30</f>
+        <v>28.390624353007297</v>
+      </c>
       <c r="K30" s="14"/>
       <c r="M30" s="1">
         <f t="shared" si="0"/>
         <v>30390.224523750003</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="12"/>
@@ -4470,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <f>'Estimate (3)'!A50</f>
         <v>8</v>
@@ -4497,7 +4515,7 @@
       </c>
       <c r="G32" s="12">
         <f>V!G65</f>
-        <v>169.53129129589973</v>
+        <v>173.73129129589972</v>
       </c>
       <c r="H32" s="12">
         <f>V!I65</f>
@@ -4505,11 +4523,11 @@
       </c>
       <c r="I32" s="12">
         <f>G32*H32</f>
-        <v>3529.6414847806327</v>
+        <v>3617.0854847806322</v>
       </c>
       <c r="J32" s="28">
         <f>I32-F32</f>
-        <v>111.18260737580067</v>
+        <v>198.62660737580018</v>
       </c>
       <c r="K32" s="14"/>
       <c r="M32" s="1">
@@ -4517,7 +4535,7 @@
         <v>4273.0735967560404</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
       <c r="B33" s="32" t="str">
         <f>'Estimate (3)'!B58</f>
@@ -4534,16 +4552,19 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12">
         <f>V!J66</f>
-        <v>101.02708710905257</v>
-      </c>
-      <c r="J33" s="28"/>
+        <v>103.52995110905256</v>
+      </c>
+      <c r="J33" s="28">
+        <f>I33-F33</f>
+        <v>5.6851857765315401</v>
+      </c>
       <c r="K33" s="14"/>
       <c r="M33" s="1">
         <f t="shared" si="0"/>
         <v>122.30595666565128</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="12"/>
@@ -4560,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f>'Estimate (3)'!A60</f>
         <v>9</v>
@@ -4586,20 +4607,20 @@
         <v>102494.07193699971</v>
       </c>
       <c r="G35" s="12">
-        <f>V!G73</f>
-        <v>6.9988592413899129</v>
+        <f>V!G74</f>
+        <v>7.2088592413899129</v>
       </c>
       <c r="H35" s="12">
-        <f>V!I73</f>
+        <f>V!I74</f>
         <v>14362.76</v>
       </c>
       <c r="I35" s="12">
         <f>G35*H35</f>
-        <v>100522.93555786539</v>
+        <v>103539.11515786538</v>
       </c>
       <c r="J35" s="28">
         <f>I35-F35</f>
-        <v>-1971.1363791343174</v>
+        <v>1045.0432208656712</v>
       </c>
       <c r="K35" s="14"/>
       <c r="M35" s="1">
@@ -4607,7 +4628,7 @@
         <v>128117.58992124963</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
       <c r="B36" s="32" t="str">
         <f>'Estimate (3)'!B67</f>
@@ -4623,17 +4644,20 @@
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12">
-        <f>V!J74</f>
-        <v>9382.1541831953036</v>
-      </c>
-      <c r="J36" s="28"/>
+        <f>V!J75</f>
+        <v>9663.6646851953028</v>
+      </c>
+      <c r="J36" s="28">
+        <f>I36-F36</f>
+        <v>97.537507951316002</v>
+      </c>
       <c r="K36" s="14"/>
       <c r="M36" s="1">
         <f t="shared" si="0"/>
         <v>11957.658971554984</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="12"/>
@@ -4650,12 +4674,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <f>'Estimate (3)'!A69</f>
         <v>10</v>
       </c>
-      <c r="B38" s="94" t="str">
+      <c r="B38" s="71" t="str">
         <f>'Estimate (3)'!B69</f>
         <v>cf/=;L=;L= nflu kmnfd] 808L sf6\g], df]8\g] #) dL6/ ;Dd</v>
       </c>
@@ -4676,11 +4700,11 @@
         <v>9329.4971045412967</v>
       </c>
       <c r="G38" s="12">
-        <f>V!G79</f>
+        <f>V!G80</f>
         <v>7.8599656583672295E-2</v>
       </c>
       <c r="H38" s="12">
-        <f>V!I79</f>
+        <f>V!I80</f>
         <v>131940</v>
       </c>
       <c r="I38" s="12">
@@ -4697,7 +4721,7 @@
         <v>11661.871380676621</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
       <c r="B39" s="32" t="str">
         <f>'Estimate (3)'!B73</f>
@@ -4713,7 +4737,7 @@
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12">
-        <f>V!J80</f>
+        <f>V!J81</f>
         <v>1085.1468587941799</v>
       </c>
       <c r="J39" s="28">
@@ -4726,7 +4750,7 @@
         <v>1220.2804023163669</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="12"/>
@@ -4743,8 +4767,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="99" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="95">
+    <row r="41" spans="1:13" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="72">
         <f>'Estimate (3)'!A75</f>
         <v>11</v>
       </c>
@@ -4752,45 +4776,45 @@
         <f>'Estimate (3)'!B75</f>
         <v>!@=% dL=dL= l;d]G6 afn'jf -!M$_ Knfi6/</v>
       </c>
-      <c r="C41" s="96" t="str">
+      <c r="C41" s="73" t="str">
         <f>'Estimate (3)'!H78</f>
         <v>sqm</v>
       </c>
-      <c r="D41" s="96">
+      <c r="D41" s="73">
         <f>'Estimate (3)'!G78</f>
         <v>44.939817128924112</v>
       </c>
-      <c r="E41" s="96">
+      <c r="E41" s="73">
         <f>'Estimate (3)'!I78</f>
         <v>405.86</v>
       </c>
-      <c r="F41" s="96">
+      <c r="F41" s="73">
         <f>D41*E41</f>
         <v>18239.27417994514</v>
       </c>
-      <c r="G41" s="96">
-        <f>V!G85</f>
-        <v>50.28</v>
-      </c>
-      <c r="H41" s="96">
-        <f>V!I85</f>
+      <c r="G41" s="73">
+        <f>V!G87</f>
+        <v>54.480000000000004</v>
+      </c>
+      <c r="H41" s="73">
+        <f>V!I87</f>
         <v>405.86</v>
       </c>
-      <c r="I41" s="96">
+      <c r="I41" s="73">
         <f>G41*H41</f>
-        <v>20406.640800000001</v>
-      </c>
-      <c r="J41" s="97">
+        <v>22111.252800000002</v>
+      </c>
+      <c r="J41" s="74">
         <f>I41-F41</f>
-        <v>2167.3666200548614</v>
-      </c>
-      <c r="K41" s="98"/>
+        <v>3871.9786200548624</v>
+      </c>
+      <c r="K41" s="75"/>
       <c r="M41" s="1">
         <f t="shared" si="0"/>
         <v>22799.092724931426</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
       <c r="B42" s="32" t="str">
         <f>'Estimate (3)'!B79</f>
@@ -4806,17 +4830,20 @@
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12">
-        <f>V!J86</f>
-        <v>729.86749680000003</v>
-      </c>
-      <c r="J42" s="28"/>
+        <f>V!J88</f>
+        <v>790.83494880000012</v>
+      </c>
+      <c r="J42" s="74">
+        <f>I42-F42</f>
+        <v>138.48586696750988</v>
+      </c>
       <c r="K42" s="14"/>
       <c r="M42" s="1">
         <f t="shared" si="0"/>
         <v>815.43635229061283</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="12"/>
@@ -4833,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <f>'Estimate (3)'!A81</f>
         <v>12</v>
@@ -4859,11 +4886,11 @@
         <v>500</v>
       </c>
       <c r="G44" s="12">
-        <f>V!C88</f>
+        <f>V!C90</f>
         <v>1</v>
       </c>
       <c r="H44" s="12">
-        <f>V!I88</f>
+        <f>V!I90</f>
         <v>500</v>
       </c>
       <c r="I44" s="12">
@@ -4880,7 +4907,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="12"/>
@@ -4893,7 +4920,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="14"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6" t="s">
         <v>16</v>
@@ -4909,16 +4936,23 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7">
         <f>SUM(I13:I44)</f>
-        <v>565521.79621734493</v>
+        <v>570675.01263534476</v>
       </c>
       <c r="J46" s="13">
         <f>I46-F46</f>
-        <v>1886.8681472097524</v>
+        <v>7040.0845652095741</v>
       </c>
       <c r="K46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4932,13 +4966,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4954,139 +4981,139 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U154"/>
+  <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
       <c r="O6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5124,7 +5151,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -5147,7 +5174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="str">
         <f>B30</f>
@@ -5182,7 +5209,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -5214,7 +5241,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -5239,7 +5266,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -5259,7 +5286,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -5283,7 +5310,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>64</v>
@@ -5310,7 +5337,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>42</v>
@@ -5335,7 +5362,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="19"/>
@@ -5348,7 +5375,7 @@
       <c r="J17" s="41"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:21" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -5365,7 +5392,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="37" t="s">
         <v>66</v>
@@ -5391,7 +5418,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37"/>
       <c r="C20" s="19">
@@ -5414,7 +5441,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -5439,7 +5466,7 @@
       </c>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="37"/>
       <c r="C22" s="19"/>
@@ -5452,7 +5479,7 @@
       <c r="J22" s="41"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -5469,7 +5496,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="37" t="str">
         <f>B15</f>
@@ -5496,7 +5523,7 @@
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>80</v>
@@ -5521,7 +5548,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37" t="s">
         <v>42</v>
@@ -5546,7 +5573,7 @@
       </c>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="37" t="s">
         <v>40</v>
@@ -5564,7 +5591,7 @@
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="37"/>
       <c r="C28" s="19"/>
@@ -5577,7 +5604,7 @@
       <c r="J28" s="41"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>5</v>
       </c>
@@ -5595,17 +5622,17 @@
       <c r="K29" s="21"/>
       <c r="M29" s="25"/>
       <c r="N29" s="1"/>
-      <c r="O29" s="85" t="s">
+      <c r="O29" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="P29" s="85"/>
-      <c r="Q29" s="85"/>
-      <c r="R29" s="85"/>
-      <c r="S29" s="85"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="85"/>
-    </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="81"/>
+      <c r="Q29" s="81"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+    </row>
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="37" t="str">
         <f>B37</f>
@@ -5640,7 +5667,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37"/>
       <c r="C31" s="36">
@@ -5672,7 +5699,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="37"/>
       <c r="C32" s="36">
@@ -5704,7 +5731,7 @@
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>42</v>
@@ -5729,7 +5756,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37" t="s">
         <v>40</v>
@@ -5747,7 +5774,7 @@
       </c>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="37"/>
       <c r="C35" s="42"/>
@@ -5760,7 +5787,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -5784,7 +5811,7 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="37" t="s">
         <v>62</v>
@@ -5803,7 +5830,7 @@
         <v>0.05</v>
       </c>
       <c r="G37" s="39">
-        <f>PRODUCT(C37:F37)</f>
+        <f t="shared" ref="G37:G42" si="1">PRODUCT(C37:F37)</f>
         <v>0.36240000000000006</v>
       </c>
       <c r="H37" s="40"/>
@@ -5818,7 +5845,7 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="37"/>
       <c r="C38" s="36">
@@ -5835,7 +5862,7 @@
         <v>0.05</v>
       </c>
       <c r="G38" s="39">
-        <f>PRODUCT(C38:F38)</f>
+        <f t="shared" si="1"/>
         <v>0.12004500000000001</v>
       </c>
       <c r="H38" s="40"/>
@@ -5850,7 +5877,7 @@
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="37" t="s">
         <v>62</v>
@@ -5869,7 +5896,7 @@
         <v>0.05</v>
       </c>
       <c r="G39" s="39">
-        <f>PRODUCT(C39:F39)</f>
+        <f t="shared" si="1"/>
         <v>0.3448</v>
       </c>
       <c r="H39" s="40"/>
@@ -5884,7 +5911,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="37"/>
       <c r="C40" s="36">
@@ -5901,7 +5928,7 @@
         <v>0.05</v>
       </c>
       <c r="G40" s="39">
-        <f>PRODUCT(C40:F40)</f>
+        <f t="shared" si="1"/>
         <v>0.11421500000000001</v>
       </c>
       <c r="H40" s="40"/>
@@ -5916,7 +5943,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="37" t="s">
         <v>62</v>
@@ -5935,7 +5962,7 @@
         <v>0.05</v>
       </c>
       <c r="G41" s="39">
-        <f>PRODUCT(C41:F41)</f>
+        <f t="shared" si="1"/>
         <v>0.31125000000000003</v>
       </c>
       <c r="H41" s="40"/>
@@ -5950,7 +5977,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="37"/>
       <c r="C42" s="36">
@@ -5967,7 +5994,7 @@
         <v>0.05</v>
       </c>
       <c r="G42" s="39">
-        <f>PRODUCT(C42:F42)</f>
+        <f t="shared" si="1"/>
         <v>0.12450000000000001</v>
       </c>
       <c r="H42" s="40"/>
@@ -5982,7 +6009,7 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="37" t="s">
         <v>73</v>
@@ -6002,7 +6029,7 @@
         <v>0.05</v>
       </c>
       <c r="G43" s="39">
-        <f t="shared" ref="G43:G44" si="1">PRODUCT(C43:F43)</f>
+        <f t="shared" ref="G43:G44" si="2">PRODUCT(C43:F43)</f>
         <v>0.24092500000000003</v>
       </c>
       <c r="H43" s="40"/>
@@ -6017,7 +6044,7 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="37"/>
       <c r="C44" s="47">
@@ -6034,7 +6061,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G44" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.36138750000000003</v>
       </c>
       <c r="H44" s="40"/>
@@ -6049,7 +6076,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="37"/>
       <c r="C45" s="47">
@@ -6066,7 +6093,7 @@
         <v>0.1</v>
       </c>
       <c r="G45" s="39">
-        <f t="shared" ref="G45:G47" si="2">PRODUCT(C45:F45)</f>
+        <f t="shared" ref="G45:G47" si="3">PRODUCT(C45:F45)</f>
         <v>0.48185000000000006</v>
       </c>
       <c r="H45" s="40"/>
@@ -6081,7 +6108,7 @@
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>80</v>
@@ -6101,7 +6128,7 @@
         <v>5.0797521080971242E-2</v>
       </c>
       <c r="G46" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.4185163327577306E-2</v>
       </c>
       <c r="H46" s="40"/>
@@ -6116,7 +6143,7 @@
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="37"/>
       <c r="C47" s="47">
@@ -6133,7 +6160,7 @@
         <v>0.4</v>
       </c>
       <c r="G47" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="H47" s="40"/>
@@ -6148,7 +6175,7 @@
       <c r="R47" s="25"/>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="37" t="s">
         <v>42</v>
@@ -6173,7 +6200,7 @@
       </c>
       <c r="K48" s="36"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="37" t="s">
         <v>40</v>
@@ -6191,7 +6218,7 @@
       </c>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="37"/>
       <c r="C50" s="42"/>
@@ -6204,7 +6231,7 @@
       <c r="J50" s="45"/>
       <c r="K50" s="36"/>
     </row>
-    <row r="51" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A51" s="63">
         <v>7</v>
       </c>
@@ -6221,7 +6248,7 @@
       <c r="J51" s="45"/>
       <c r="K51" s="29"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="37" t="s">
         <v>62</v>
@@ -6256,7 +6283,7 @@
       <c r="R52" s="25"/>
       <c r="S52" s="25"/>
     </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="37"/>
       <c r="C53" s="36">
@@ -6270,11 +6297,11 @@
         <v>1.04</v>
       </c>
       <c r="F53" s="38">
-        <f t="shared" ref="F53:F54" si="3">2.7-0.05-0.1</f>
+        <f t="shared" ref="F53:F54" si="4">2.7-0.05-0.1</f>
         <v>2.5500000000000003</v>
       </c>
       <c r="G53" s="39">
-        <f t="shared" ref="G53:G54" si="4">PRODUCT(C53:F53)</f>
+        <f t="shared" ref="G53:G54" si="5">PRODUCT(C53:F53)</f>
         <v>11.430120000000002</v>
       </c>
       <c r="H53" s="40"/>
@@ -6289,7 +6316,7 @@
       <c r="R53" s="25"/>
       <c r="S53" s="25"/>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="37"/>
       <c r="C54" s="36">
@@ -6303,11 +6330,11 @@
         <v>1.05</v>
       </c>
       <c r="F54" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5500000000000003</v>
       </c>
       <c r="G54" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.111625000000004</v>
       </c>
       <c r="H54" s="40"/>
@@ -6322,7 +6349,7 @@
       <c r="R54" s="25"/>
       <c r="S54" s="25"/>
     </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="37" t="s">
         <v>42</v>
@@ -6347,7 +6374,7 @@
       </c>
       <c r="K55" s="36"/>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="37" t="s">
         <v>40</v>
@@ -6365,7 +6392,7 @@
       </c>
       <c r="K56" s="36"/>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="37"/>
       <c r="C57" s="42"/>
@@ -6378,7 +6405,7 @@
       <c r="J57" s="44"/>
       <c r="K57" s="36"/>
     </row>
-    <row r="58" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
         <v>8</v>
       </c>
@@ -6395,7 +6422,7 @@
       <c r="J58" s="41"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="37" t="s">
         <v>56</v>
@@ -6413,7 +6440,7 @@
         <v>2.7430661383724475</v>
       </c>
       <c r="G59" s="39">
-        <f t="shared" ref="G59:G63" si="5">PRODUCT(C59:F59)</f>
+        <f t="shared" ref="G59:G63" si="6">PRODUCT(C59:F59)</f>
         <v>65.7683757516632</v>
       </c>
       <c r="H59" s="40"/>
@@ -6421,7 +6448,7 @@
       <c r="J59" s="40"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="37"/>
       <c r="C60" s="36">
@@ -6437,7 +6464,7 @@
         <v>2.5906735751295336</v>
       </c>
       <c r="G60" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.772312876934713</v>
       </c>
       <c r="H60" s="40"/>
@@ -6445,7 +6472,7 @@
       <c r="J60" s="40"/>
       <c r="K60" s="21"/>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="37" t="s">
         <v>59</v>
@@ -6463,7 +6490,7 @@
         <v>2.1334958854007922</v>
       </c>
       <c r="G61" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3.9015468797332375</v>
       </c>
       <c r="H61" s="40"/>
@@ -6471,7 +6498,7 @@
       <c r="J61" s="40"/>
       <c r="K61" s="21"/>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="37"/>
       <c r="C62" s="36">
@@ -6487,7 +6514,7 @@
         <v>1.8287107589149649</v>
       </c>
       <c r="G62" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.786819199809456</v>
       </c>
       <c r="H62" s="40"/>
@@ -6495,7 +6522,7 @@
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="37" t="s">
         <v>60</v>
@@ -6513,7 +6540,7 @@
         <v>1.2191405059433098</v>
       </c>
       <c r="G63" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.6010312531554916</v>
       </c>
       <c r="H63" s="40"/>
@@ -6521,7 +6548,7 @@
       <c r="J63" s="40"/>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="37" t="s">
         <v>76</v>
@@ -6533,15 +6560,15 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="39">
-        <f>G85</f>
-        <v>50.28</v>
+        <f>G87</f>
+        <v>54.480000000000004</v>
       </c>
       <c r="H64" s="40"/>
       <c r="I64" s="40"/>
       <c r="J64" s="40"/>
       <c r="K64" s="21"/>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="37" t="s">
         <v>42</v>
@@ -6552,7 +6579,7 @@
       <c r="F65" s="21"/>
       <c r="G65" s="23">
         <f>SUM(G59:G64)</f>
-        <v>169.53129129589973</v>
+        <v>173.73129129589972</v>
       </c>
       <c r="H65" s="22" t="s">
         <v>57</v>
@@ -6562,11 +6589,11 @@
       </c>
       <c r="J65" s="41">
         <f>G65*I65</f>
-        <v>3529.6414847806327</v>
+        <v>3617.0854847806322</v>
       </c>
       <c r="K65" s="21"/>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="37" t="s">
         <v>40</v>
@@ -6580,11 +6607,11 @@
       <c r="I66" s="23"/>
       <c r="J66" s="41">
         <f>0.13*G65*458.4/100</f>
-        <v>101.02708710905257</v>
+        <v>103.52995110905256</v>
       </c>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
       <c r="B67" s="37"/>
       <c r="C67" s="19"/>
@@ -6597,7 +6624,7 @@
       <c r="J67" s="41"/>
       <c r="K67" s="21"/>
     </row>
-    <row r="68" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="30" x14ac:dyDescent="0.3">
       <c r="A68" s="18">
         <v>9</v>
       </c>
@@ -6618,7 +6645,7 @@
         <v>37.665999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="37" t="s">
         <v>56</v>
@@ -6627,7 +6654,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="38">
-        <f>3.92+3.94+3.52+3.49+3.98+2.1</f>
+        <f>3.92+3.94+(3.52+3.49)+3.98+2.1</f>
         <v>20.95</v>
       </c>
       <c r="E69" s="38">
@@ -6658,7 +6685,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="B70" s="37"/>
       <c r="C70" s="47">
@@ -6683,7 +6710,7 @@
       <c r="J70" s="40"/>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="37" t="s">
         <v>79</v>
@@ -6710,7 +6737,7 @@
       <c r="J71" s="40"/>
       <c r="K71" s="21"/>
     </row>
-    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="37" t="s">
         <v>78</v>
@@ -6739,56 +6766,62 @@
       <c r="J72" s="40"/>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="23">
-        <f>SUM(G69:G72)</f>
-        <v>6.9988592413899129</v>
-      </c>
-      <c r="H73" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I73" s="23">
-        <v>14362.76</v>
-      </c>
-      <c r="J73" s="41">
-        <f>G73*I73</f>
-        <v>100522.93555786539</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C73" s="47">
+        <v>1</v>
+      </c>
+      <c r="D73" s="38">
+        <v>3</v>
+      </c>
+      <c r="E73" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="F73" s="38">
+        <v>0.7</v>
+      </c>
+      <c r="G73" s="39">
+        <f>PRODUCT(C73:F73)</f>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="H73" s="40"/>
+      <c r="I73" s="40"/>
+      <c r="J73" s="40"/>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="20"/>
       <c r="E74" s="21"/>
       <c r="F74" s="21"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="23"/>
+      <c r="G74" s="23">
+        <f>SUM(G69:G73)</f>
+        <v>7.2088592413899129</v>
+      </c>
+      <c r="H74" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" s="23">
+        <v>14362.76</v>
+      </c>
       <c r="J74" s="41">
-        <f>0.13*G73*10311.74</f>
-        <v>9382.1541831953036</v>
+        <f>G74*I74</f>
+        <v>103539.11515786538</v>
       </c>
       <c r="K74" s="21"/>
-      <c r="M74">
-        <f>14/3.281</f>
-        <v>4.2669917708015843</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="18"/>
-      <c r="B75" s="37"/>
+      <c r="B75" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C75" s="19"/>
       <c r="D75" s="20"/>
       <c r="E75" s="21"/>
@@ -6796,141 +6829,145 @@
       <c r="G75" s="23"/>
       <c r="H75" s="22"/>
       <c r="I75" s="23"/>
-      <c r="J75" s="41"/>
+      <c r="J75" s="41">
+        <f>0.13*G74*10311.74</f>
+        <v>9663.6646851953028</v>
+      </c>
       <c r="K75" s="21"/>
-    </row>
-    <row r="76" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="18">
-        <v>10</v>
-      </c>
-      <c r="B76" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="E76" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="F76" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" s="68" t="s">
-        <v>70</v>
-      </c>
+      <c r="M75">
+        <f>14/3.281</f>
+        <v>4.2669917708015843</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="18"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="22"/>
       <c r="I76" s="23"/>
       <c r="J76" s="41"/>
       <c r="K76" s="21"/>
     </row>
-    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
-      <c r="B77" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C77" s="19">
-        <v>4</v>
-      </c>
-      <c r="D77" s="20">
-        <f>3.92+3.94+3.52+3.49+3.98+2.1</f>
-        <v>20.95</v>
-      </c>
-      <c r="E77" s="21">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
-      </c>
-      <c r="F77" s="21">
-        <f>PRODUCT(C77:E77)</f>
-        <v>51.728395061728392</v>
-      </c>
-      <c r="G77" s="69">
-        <f>F77/1000</f>
-        <v>5.172839506172839E-2</v>
+    <row r="77" spans="1:16" ht="30" x14ac:dyDescent="0.3">
+      <c r="A77" s="18">
+        <v>10</v>
+      </c>
+      <c r="B77" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="F77" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G77" s="68" t="s">
+        <v>70</v>
       </c>
       <c r="H77" s="22"/>
       <c r="I77" s="23"/>
       <c r="J77" s="41"/>
       <c r="K77" s="21"/>
     </row>
-    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C78" s="19">
-        <f>2*TRUNC(D77/(8/12/3.281),0)</f>
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="D78" s="20">
-        <f>(7+3+3)/12/3.281</f>
-        <v>0.33018388702631307</v>
+        <f>3.92+3.94+3.52+3.49+3.98+2.1</f>
+        <v>20.95</v>
       </c>
       <c r="E78" s="21">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
       </c>
       <c r="F78" s="21">
         <f>PRODUCT(C78:E78)</f>
-        <v>26.871261521943897</v>
+        <v>51.728395061728392</v>
       </c>
       <c r="G78" s="69">
         <f>F78/1000</f>
-        <v>2.6871261521943898E-2</v>
+        <v>5.172839506172839E-2</v>
       </c>
       <c r="H78" s="22"/>
       <c r="I78" s="23"/>
       <c r="J78" s="41"/>
       <c r="K78" s="21"/>
     </row>
-    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C79" s="19"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="23">
-        <f>SUM(G77:G78)</f>
-        <v>7.8599656583672295E-2</v>
-      </c>
-      <c r="H79" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I79" s="23">
-        <v>131940</v>
-      </c>
-      <c r="J79" s="41">
-        <f>G79*I79</f>
-        <v>10370.438689649722</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C79" s="19">
+        <f>2*TRUNC(D78/(8/12/3.281),0)</f>
+        <v>206</v>
+      </c>
+      <c r="D79" s="20">
+        <f>(7+3+3)/12/3.281</f>
+        <v>0.33018388702631307</v>
+      </c>
+      <c r="E79" s="21">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F79" s="21">
+        <f>PRODUCT(C79:E79)</f>
+        <v>26.871261521943897</v>
+      </c>
+      <c r="G79" s="69">
+        <f>F79/1000</f>
+        <v>2.6871261521943898E-2</v>
+      </c>
+      <c r="H79" s="22"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="41"/>
       <c r="K79" s="21"/>
     </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
       <c r="B80" s="37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="20"/>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="23"/>
+      <c r="G80" s="23">
+        <f>SUM(G78:G79)</f>
+        <v>7.8599656583672295E-2</v>
+      </c>
+      <c r="H80" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I80" s="23">
+        <v>131940</v>
+      </c>
       <c r="J80" s="41">
-        <f>0.13*G79*106200</f>
-        <v>1085.1468587941799</v>
+        <f>G80*I80</f>
+        <v>10370.438689649722</v>
       </c>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18"/>
-      <c r="B81" s="37"/>
+      <c r="B81" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C81" s="19"/>
       <c r="D81" s="20"/>
       <c r="E81" s="21"/>
@@ -6938,16 +6975,15 @@
       <c r="G81" s="23"/>
       <c r="H81" s="22"/>
       <c r="I81" s="23"/>
-      <c r="J81" s="41"/>
+      <c r="J81" s="41">
+        <f>0.13*G80*106200</f>
+        <v>1085.1468587941799</v>
+      </c>
       <c r="K81" s="21"/>
     </row>
-    <row r="82" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="18">
-        <v>11</v>
-      </c>
-      <c r="B82" s="70" t="s">
-        <v>74</v>
-      </c>
+    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="18"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="19"/>
       <c r="D82" s="20"/>
       <c r="E82" s="21"/>
@@ -6958,149 +6994,143 @@
       <c r="J82" s="41"/>
       <c r="K82" s="21"/>
     </row>
-    <row r="83" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
-      <c r="B83" s="37" t="s">
+    <row r="83" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="18">
+        <v>11</v>
+      </c>
+      <c r="B83" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" s="19"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="41"/>
+      <c r="K83" s="21"/>
+    </row>
+    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="18"/>
+      <c r="B84" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C83" s="36">
+      <c r="C84" s="36">
         <v>1</v>
       </c>
-      <c r="D83" s="38">
+      <c r="D84" s="38">
         <f>3.92+3.94+0.23+0.23+3.52+3.49+3.98+0.23+0.23+2.1</f>
         <v>21.87</v>
-      </c>
-      <c r="E83" s="38"/>
-      <c r="F83" s="38">
-        <v>1.2</v>
-      </c>
-      <c r="G83" s="39">
-        <f t="shared" ref="G83:G84" si="6">PRODUCT(C83:F83)</f>
-        <v>26.244</v>
-      </c>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40"/>
-      <c r="K83" s="21"/>
-    </row>
-    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="36">
-        <v>1</v>
-      </c>
-      <c r="D84" s="38">
-        <f>3.92-0.23+3.94+3.52+3.49-0.23-0.23+3.98+2.1-0.23</f>
-        <v>20.03</v>
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38">
         <v>1.2</v>
       </c>
       <c r="G84" s="39">
-        <f t="shared" si="6"/>
-        <v>24.036000000000001</v>
+        <f t="shared" ref="G84:G86" si="7">PRODUCT(C84:F84)</f>
+        <v>26.244</v>
       </c>
       <c r="H84" s="40"/>
       <c r="I84" s="40"/>
       <c r="J84" s="40"/>
       <c r="K84" s="21"/>
     </row>
-    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18"/>
-      <c r="B85" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="23">
-        <f>SUM(G83:G84)</f>
-        <v>50.28</v>
-      </c>
-      <c r="H85" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I85" s="23">
-        <v>405.86</v>
-      </c>
-      <c r="J85" s="41">
-        <f>G85*I85</f>
-        <v>20406.640800000001</v>
-      </c>
+      <c r="B85" s="37"/>
+      <c r="C85" s="36">
+        <v>1</v>
+      </c>
+      <c r="D85" s="38">
+        <f>3.92-0.23+3.94+3.52+3.49-0.23-0.23+3.98+2.1-0.23</f>
+        <v>20.03</v>
+      </c>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G85" s="39">
+        <f t="shared" si="7"/>
+        <v>24.036000000000001</v>
+      </c>
+      <c r="H85" s="40"/>
+      <c r="I85" s="40"/>
+      <c r="J85" s="40"/>
       <c r="K85" s="21"/>
     </row>
-    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18"/>
       <c r="B86" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C86" s="19"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="23"/>
-      <c r="H86" s="22"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="41">
-        <f>0.13*G85*11166.2/100</f>
-        <v>729.86749680000003</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C86" s="36">
+        <v>2</v>
+      </c>
+      <c r="D86" s="38">
+        <f>D73</f>
+        <v>3</v>
+      </c>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38">
+        <f>F73</f>
+        <v>0.7</v>
+      </c>
+      <c r="G86" s="39">
+        <f t="shared" si="7"/>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="H86" s="40"/>
+      <c r="I86" s="40"/>
+      <c r="J86" s="40"/>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18"/>
-      <c r="B87" s="37"/>
+      <c r="B87" s="37" t="s">
+        <v>42</v>
+      </c>
       <c r="C87" s="19"/>
       <c r="D87" s="20"/>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
-      <c r="G87" s="23"/>
-      <c r="H87" s="22"/>
-      <c r="I87" s="23"/>
-      <c r="J87" s="41"/>
+      <c r="G87" s="23">
+        <f>SUM(G84:G86)</f>
+        <v>54.480000000000004</v>
+      </c>
+      <c r="H87" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I87" s="23">
+        <v>405.86</v>
+      </c>
+      <c r="J87" s="41">
+        <f>G87*I87</f>
+        <v>22111.252800000002</v>
+      </c>
       <c r="K87" s="21"/>
     </row>
-    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18">
-        <v>12</v>
-      </c>
-      <c r="B88" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C88" s="19">
-        <v>1</v>
-      </c>
+    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="18"/>
+      <c r="B88" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="19"/>
       <c r="D88" s="20"/>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
-      <c r="G88" s="34">
-        <f t="shared" ref="G88" si="7">PRODUCT(C88:F88)</f>
-        <v>1</v>
-      </c>
-      <c r="H88" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I88" s="23">
-        <v>500</v>
-      </c>
-      <c r="J88" s="34">
-        <f>G88*I88</f>
-        <v>500</v>
+      <c r="G88" s="23"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="41">
+        <f>0.13*G87*11166.2/100</f>
+        <v>790.83494880000012</v>
       </c>
       <c r="K88" s="21"/>
-      <c r="M88" s="25"/>
-      <c r="N88" s="1"/>
-      <c r="O88" s="1"/>
-      <c r="P88" s="1"/>
-      <c r="Q88" s="1"/>
-      <c r="R88" s="25"/>
-      <c r="S88" s="25"/>
-    </row>
-    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="18"/>
-      <c r="B89" s="24"/>
+      <c r="B89" s="37"/>
       <c r="C89" s="19"/>
       <c r="D89" s="20"/>
       <c r="E89" s="21"/>
@@ -7110,120 +7140,127 @@
       <c r="I89" s="23"/>
       <c r="J89" s="41"/>
       <c r="K89" s="21"/>
-      <c r="M89" s="25"/>
-      <c r="N89" s="1">
+    </row>
+    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="18">
+        <v>12</v>
+      </c>
+      <c r="B90" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C90" s="19">
+        <v>1</v>
+      </c>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="34">
+        <f t="shared" ref="G90" si="8">PRODUCT(C90:F90)</f>
+        <v>1</v>
+      </c>
+      <c r="H90" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I90" s="23">
+        <v>500</v>
+      </c>
+      <c r="J90" s="34">
+        <f>G90*I90</f>
+        <v>500</v>
+      </c>
+      <c r="K90" s="21"/>
+      <c r="M90" s="25"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="25"/>
+      <c r="S90" s="25"/>
+    </row>
+    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="18"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="23"/>
+      <c r="J91" s="41"/>
+      <c r="K91" s="21"/>
+      <c r="M91" s="25"/>
+      <c r="N91" s="1">
         <f>2.4*3.281</f>
         <v>7.8743999999999996</v>
       </c>
-      <c r="O89" s="1"/>
-      <c r="P89" s="1"/>
-      <c r="Q89" s="1"/>
-      <c r="R89" s="25"/>
-      <c r="S89" s="25"/>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A90" s="40"/>
-      <c r="B90" s="46" t="s">
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="25"/>
+      <c r="S91" s="25"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A92" s="40"/>
+      <c r="B92" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C90" s="47"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="41"/>
-      <c r="H90" s="41"/>
-      <c r="I90" s="41"/>
-      <c r="J90" s="41">
-        <f>SUM(J10:J88)</f>
-        <v>565521.79621734493</v>
-      </c>
-      <c r="K90" s="36"/>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A91" s="58"/>
-      <c r="B91" s="61"/>
-      <c r="C91" s="62"/>
-      <c r="D91" s="59"/>
-      <c r="E91" s="59"/>
-      <c r="F91" s="59"/>
-      <c r="G91" s="60"/>
-      <c r="H91" s="60"/>
-      <c r="I91" s="60"/>
-      <c r="J91" s="60"/>
-      <c r="K91" s="57"/>
-    </row>
-    <row r="92" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
-      <c r="B92" s="29" t="s">
+      <c r="C92" s="47"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="41">
+        <f>SUM(J10:J90)</f>
+        <v>570675.01263534476</v>
+      </c>
+      <c r="K92" s="36"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A93" s="58"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="62"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="59"/>
+      <c r="F93" s="59"/>
+      <c r="G93" s="60"/>
+      <c r="H93" s="60"/>
+      <c r="I93" s="60"/>
+      <c r="J93" s="60"/>
+      <c r="K93" s="57"/>
+    </row>
+    <row r="94" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="50"/>
+      <c r="B94" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C92" s="90">
-        <f>J90</f>
-        <v>565521.79621734493</v>
-      </c>
-      <c r="D92" s="90"/>
-      <c r="E92" s="39">
+      <c r="C94" s="77">
+        <f>J92</f>
+        <v>570675.01263534476</v>
+      </c>
+      <c r="D94" s="77"/>
+      <c r="E94" s="39">
         <v>100</v>
       </c>
-      <c r="F92" s="51"/>
-      <c r="G92" s="52"/>
-      <c r="H92" s="51"/>
-      <c r="I92" s="53"/>
-      <c r="J92" s="54"/>
-      <c r="K92" s="55"/>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="56"/>
-      <c r="B93" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" s="93">
-        <v>500000</v>
-      </c>
-      <c r="D93" s="93"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="49"/>
-      <c r="G93" s="48"/>
-      <c r="H93" s="48"/>
-      <c r="I93" s="48"/>
-      <c r="J93" s="48"/>
-      <c r="K93" s="49"/>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A94" s="56"/>
-      <c r="B94" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C94" s="93">
-        <f>C93-C96-C97</f>
-        <v>475000</v>
-      </c>
-      <c r="D94" s="93"/>
-      <c r="E94" s="39">
-        <f>C94/C92*100</f>
-        <v>83.993225933496106</v>
-      </c>
-      <c r="F94" s="49"/>
-      <c r="G94" s="48"/>
-      <c r="H94" s="48"/>
-      <c r="I94" s="48"/>
-      <c r="J94" s="48"/>
-      <c r="K94" s="49"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F94" s="51"/>
+      <c r="G94" s="52"/>
+      <c r="H94" s="51"/>
+      <c r="I94" s="53"/>
+      <c r="J94" s="54"/>
+      <c r="K94" s="55"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="56"/>
       <c r="B95" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C95" s="90">
-        <f>C92-C94</f>
-        <v>90521.796217344934</v>
-      </c>
-      <c r="D95" s="90"/>
-      <c r="E95" s="39">
-        <f>100-E94</f>
-        <v>16.006774066503894</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C95" s="80">
+        <v>500000</v>
+      </c>
+      <c r="D95" s="80"/>
+      <c r="E95" s="39"/>
       <c r="F95" s="49"/>
       <c r="G95" s="48"/>
       <c r="H95" s="48"/>
@@ -7231,18 +7268,19 @@
       <c r="J95" s="48"/>
       <c r="K95" s="49"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="56"/>
       <c r="B96" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C96" s="90">
-        <f>C93*0.03</f>
-        <v>15000</v>
-      </c>
-      <c r="D96" s="90"/>
+        <v>33</v>
+      </c>
+      <c r="C96" s="80">
+        <f>C95-C98-C99</f>
+        <v>475000</v>
+      </c>
+      <c r="D96" s="80"/>
       <c r="E96" s="39">
-        <v>3</v>
+        <f>C96/C94*100</f>
+        <v>83.234764004556112</v>
       </c>
       <c r="F96" s="49"/>
       <c r="G96" s="48"/>
@@ -7251,18 +7289,19 @@
       <c r="J96" s="48"/>
       <c r="K96" s="49"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="56"/>
       <c r="B97" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C97" s="90">
-        <f>C93*0.02</f>
-        <v>10000</v>
-      </c>
-      <c r="D97" s="90"/>
+        <v>34</v>
+      </c>
+      <c r="C97" s="77">
+        <f>C94-C96</f>
+        <v>95675.012635344756</v>
+      </c>
+      <c r="D97" s="77"/>
       <c r="E97" s="39">
-        <v>2</v>
+        <f>100-E96</f>
+        <v>16.765235995443888</v>
       </c>
       <c r="F97" s="49"/>
       <c r="G97" s="48"/>
@@ -7271,86 +7310,121 @@
       <c r="J97" s="48"/>
       <c r="K97" s="49"/>
     </row>
-    <row r="98" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="57"/>
-      <c r="B98" s="57"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="57"/>
-      <c r="E98" s="57"/>
-      <c r="F98" s="57"/>
-      <c r="G98" s="57"/>
-      <c r="H98" s="57"/>
-      <c r="I98" s="57"/>
-      <c r="J98" s="57"/>
-      <c r="K98" s="57"/>
-    </row>
-    <row r="99" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="56"/>
+      <c r="B98" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="77">
+        <f>C95*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D98" s="77"/>
+      <c r="E98" s="39">
+        <v>3</v>
+      </c>
+      <c r="F98" s="49"/>
+      <c r="G98" s="48"/>
+      <c r="H98" s="48"/>
+      <c r="I98" s="48"/>
+      <c r="J98" s="48"/>
+      <c r="K98" s="49"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="56"/>
+      <c r="B99" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" s="77">
+        <f>C95*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D99" s="77"/>
+      <c r="E99" s="39">
+        <v>2</v>
+      </c>
+      <c r="F99" s="49"/>
+      <c r="G99" s="48"/>
+      <c r="H99" s="48"/>
+      <c r="I99" s="48"/>
+      <c r="J99" s="48"/>
+      <c r="K99" s="49"/>
+    </row>
+    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="57"/>
+      <c r="B100" s="57"/>
+      <c r="C100" s="57"/>
+      <c r="D100" s="57"/>
+      <c r="E100" s="57"/>
+      <c r="F100" s="57"/>
+      <c r="G100" s="57"/>
+      <c r="H100" s="57"/>
+      <c r="I100" s="57"/>
+      <c r="J100" s="57"/>
+      <c r="K100" s="57"/>
+    </row>
+    <row r="101" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O29:U29"/>
+    <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="O29:U29"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -7358,6 +7432,11 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
little done for ganapati bill
</commit_message>
<xml_diff>
--- a/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
+++ b/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
@@ -41,7 +41,8 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Estimate (3)'!$A$1:$K$90</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$99</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Estimate (3)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
@@ -125,29 +126,7 @@
     <author>DELL</author>
   </authors>
   <commentList>
-    <comment ref="B64" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>DELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-item no. 10</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D69" authorId="0" shapeId="0">
+    <comment ref="D67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="89">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -422,6 +401,27 @@
   </si>
   <si>
     <t>-partition</t>
+  </si>
+  <si>
+    <t>Date:2081/12/06</t>
+  </si>
+  <si>
+    <t>Detail Valuated Sheet</t>
+  </si>
+  <si>
+    <t>Total Valuated</t>
+  </si>
+  <si>
+    <t>Excavator</t>
+  </si>
+  <si>
+    <t>VAT 13%</t>
+  </si>
+  <si>
+    <t>Total amount w/o VAT</t>
+  </si>
+  <si>
+    <t>Skilled</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -811,6 +811,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -821,25 +842,19 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,21 +878,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1496,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U147"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,116 +1537,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="83" t="s">
+      <c r="H6" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
       <c r="O6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2162,15 +2184,15 @@
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="81" t="s">
+      <c r="O30" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="81"/>
-      <c r="S30" s="81"/>
-      <c r="T30" s="81"/>
-      <c r="U30" s="81"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
+      <c r="S30" s="77"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="77"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
@@ -3461,11 +3483,11 @@
       <c r="B85" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C85" s="77">
+      <c r="C85" s="84">
         <f>J83</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D85" s="77"/>
+      <c r="D85" s="84"/>
       <c r="E85" s="39">
         <v>100</v>
       </c>
@@ -3481,10 +3503,10 @@
       <c r="B86" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="80">
+      <c r="C86" s="87">
         <v>500000</v>
       </c>
-      <c r="D86" s="80"/>
+      <c r="D86" s="87"/>
       <c r="E86" s="39"/>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -3498,11 +3520,11 @@
       <c r="B87" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="80">
+      <c r="C87" s="87">
         <f>C86-C89-C90</f>
         <v>475000</v>
       </c>
-      <c r="D87" s="80"/>
+      <c r="D87" s="87"/>
       <c r="E87" s="39">
         <f>C87/C85*100</f>
         <v>84.274408192973809</v>
@@ -3519,11 +3541,11 @@
       <c r="B88" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C88" s="77">
+      <c r="C88" s="84">
         <f>C85-C87</f>
         <v>88634.928070135182</v>
       </c>
-      <c r="D88" s="77"/>
+      <c r="D88" s="84"/>
       <c r="E88" s="39">
         <f>100-E87</f>
         <v>15.725591807026191</v>
@@ -3540,11 +3562,11 @@
       <c r="B89" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="77">
+      <c r="C89" s="84">
         <f>C86*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D89" s="77"/>
+      <c r="D89" s="84"/>
       <c r="E89" s="39">
         <v>3</v>
       </c>
@@ -3560,11 +3582,11 @@
       <c r="B90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="77">
+      <c r="C90" s="84">
         <f>C86*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D90" s="77"/>
+      <c r="D90" s="84"/>
       <c r="E90" s="39">
         <v>2</v>
       </c>
@@ -3646,6 +3668,14 @@
     <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
     <mergeCell ref="O30:U30"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
@@ -3654,14 +3684,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -3674,18 +3696,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -3695,91 +3717,91 @@
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-    </row>
-    <row r="2" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="98" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+    </row>
+    <row r="2" spans="1:14" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-    </row>
-    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="99" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+    </row>
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-    </row>
-    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+    </row>
+    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="95">
+      <c r="C6" s="88">
         <f>F46</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D6" s="96"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3787,90 +3809,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="95">
+      <c r="J6" s="88">
         <f>I46</f>
-        <v>570675.01263534476</v>
-      </c>
-      <c r="K6" s="96"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>564688.31314685999</v>
+      </c>
+      <c r="K6" s="89"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="I7" s="91" t="s">
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="I7" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="e">
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="78" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="I8" s="92" t="s">
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="I8" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="93" t="e">
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="98" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="I9" s="92" t="s">
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="I9" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="88" t="s">
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94" t="s">
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="88" t="s">
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="89" t="s">
+      <c r="K11" s="94" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="93"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="93"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3889,10 +3911,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="88"/>
-      <c r="K12" s="89"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.3">
+      <c r="J12" s="93"/>
+      <c r="K12" s="94"/>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <f>'Estimate (3)'!A9</f>
         <v>1</v>
@@ -3919,7 +3941,7 @@
       </c>
       <c r="G13" s="12">
         <f>V!G11</f>
-        <v>28.058400000000006</v>
+        <v>20.784000000000002</v>
       </c>
       <c r="H13" s="12">
         <f>V!I11</f>
@@ -3927,21 +3949,25 @@
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>1813.4143920000004</v>
+        <v>1343.26992</v>
       </c>
       <c r="J13" s="28">
         <f>I13-F13</f>
-        <v>669.46339200000034</v>
+        <v>199.31891999999993</v>
       </c>
       <c r="K13" s="14"/>
       <c r="M13" s="1">
         <f>1.25*F13</f>
         <v>1429.93875</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N13" s="1" t="b">
+        <f>IF(M13&gt;I13,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
-      <c r="B14" s="32" t="str">
+      <c r="B14" s="100" t="str">
         <f>'Estimate (3)'!B12</f>
         <v>VAT calculation</v>
       </c>
@@ -3956,19 +3982,23 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12">
         <f>V!J12</f>
-        <v>195.38934480000006</v>
+        <v>144.73284800000002</v>
       </c>
       <c r="J14" s="28">
         <f>I14-F14</f>
-        <v>72.13244480000003</v>
+        <v>21.475947999999988</v>
       </c>
       <c r="K14" s="14"/>
       <c r="M14" s="1">
         <f t="shared" ref="M14:M44" si="0">1.25*F14</f>
         <v>154.07112500000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="1" t="b">
+        <f t="shared" ref="N14:N44" si="1">IF(M14&gt;I14,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -3980,12 +4010,8 @@
       <c r="I15" s="12"/>
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
-      <c r="M15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>'Estimate (3)'!A14</f>
         <v>2</v>
@@ -4031,8 +4057,12 @@
         <f t="shared" si="0"/>
         <v>4355.6253171670223</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -4047,12 +4077,8 @@
         <v>0</v>
       </c>
       <c r="K17" s="14"/>
-      <c r="M17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <f>'Estimate (3)'!A19</f>
         <v>3</v>
@@ -4098,8 +4124,12 @@
         <f t="shared" si="0"/>
         <v>195.49218378543131</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="12"/>
@@ -4111,12 +4141,8 @@
       <c r="I19" s="12"/>
       <c r="J19" s="28"/>
       <c r="K19" s="14"/>
-      <c r="M19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f>'Estimate (3)'!A24</f>
         <v>4</v>
@@ -4143,7 +4169,7 @@
       </c>
       <c r="G20" s="12">
         <f>V!G26</f>
-        <v>9.3957691252666855</v>
+        <v>6.7425691252666873</v>
       </c>
       <c r="H20" s="12">
         <f>V!I26</f>
@@ -4151,21 +4177,25 @@
       </c>
       <c r="I20" s="12">
         <f>G20*H20</f>
-        <v>9536.4237890719287</v>
+        <v>6843.5053850719296</v>
       </c>
       <c r="J20" s="28">
         <f>I20-F20</f>
-        <v>2427.3029204343175</v>
+        <v>-265.61548356568164</v>
       </c>
       <c r="K20" s="14"/>
       <c r="M20" s="1">
         <f t="shared" si="0"/>
         <v>8886.4010857970134</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N20" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
-      <c r="B21" s="32" t="str">
+      <c r="B21" s="100" t="str">
         <f>'Estimate (3)'!B28</f>
         <v>VAT calculation</v>
       </c>
@@ -4180,19 +4210,23 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12">
         <f>V!J27</f>
-        <v>1052.5478821812251</v>
+        <v>755.32686666122538</v>
       </c>
       <c r="J21" s="28">
         <f>I21-F21</f>
-        <v>267.90467840188933</v>
+        <v>-29.316337118110368</v>
       </c>
       <c r="K21" s="14"/>
       <c r="M21" s="1">
         <f t="shared" si="0"/>
         <v>980.80400472416966</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="12"/>
@@ -4204,12 +4238,8 @@
       <c r="I22" s="12"/>
       <c r="J22" s="28"/>
       <c r="K22" s="14"/>
-      <c r="M22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <f>'Estimate (3)'!A30</f>
         <v>5</v>
@@ -4255,10 +4285,14 @@
         <f t="shared" si="0"/>
         <v>14717.063250000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N23" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
-      <c r="B24" s="32" t="str">
+      <c r="B24" s="100" t="str">
         <f>'Estimate (3)'!B33</f>
         <v>VAT calculation</v>
       </c>
@@ -4284,8 +4318,12 @@
         <f t="shared" si="0"/>
         <v>1278.5736600000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="12"/>
@@ -4297,12 +4335,8 @@
       <c r="I25" s="12"/>
       <c r="J25" s="28"/>
       <c r="K25" s="14"/>
-      <c r="M25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <f>'Estimate (3)'!A35</f>
         <v>6</v>
@@ -4348,10 +4382,14 @@
         <f t="shared" si="0"/>
         <v>37921.213820481564</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N26" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
-      <c r="B27" s="32" t="str">
+      <c r="B27" s="100" t="str">
         <f>'Estimate (3)'!B43</f>
         <v>VAT calculation</v>
       </c>
@@ -4377,8 +4415,12 @@
         <f t="shared" si="0"/>
         <v>3740.7224980225546</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N27" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="12"/>
@@ -4390,12 +4432,8 @@
       <c r="I28" s="12"/>
       <c r="J28" s="28"/>
       <c r="K28" s="14"/>
-      <c r="M28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <f>'Estimate (3)'!A45</f>
         <v>7</v>
@@ -4441,10 +4479,14 @@
         <f t="shared" si="0"/>
         <v>418901.22056250001</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N29" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
-      <c r="B30" s="32" t="str">
+      <c r="B30" s="100" t="str">
         <f>'Estimate (3)'!B48</f>
         <v>VAT calculation</v>
       </c>
@@ -4470,8 +4512,12 @@
         <f t="shared" si="0"/>
         <v>30390.224523750003</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="12"/>
@@ -4483,12 +4529,8 @@
       <c r="I31" s="12"/>
       <c r="J31" s="28"/>
       <c r="K31" s="14"/>
-      <c r="M31" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <f>'Estimate (3)'!A50</f>
         <v>8</v>
@@ -4514,30 +4556,34 @@
         <v>3418.458877404832</v>
       </c>
       <c r="G32" s="12">
-        <f>V!G65</f>
-        <v>173.73129129589972</v>
+        <f>V!G63</f>
+        <v>58.12761421058562</v>
       </c>
       <c r="H32" s="12">
-        <f>V!I65</f>
+        <f>V!I63</f>
         <v>20.82</v>
       </c>
       <c r="I32" s="12">
         <f>G32*H32</f>
-        <v>3617.0854847806322</v>
+        <v>1210.2169278643926</v>
       </c>
       <c r="J32" s="28">
         <f>I32-F32</f>
-        <v>198.62660737580018</v>
+        <v>-2208.2419495404392</v>
       </c>
       <c r="K32" s="14"/>
       <c r="M32" s="1">
         <f t="shared" si="0"/>
         <v>4273.0735967560404</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N32" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
-      <c r="B33" s="32" t="str">
+      <c r="B33" s="100" t="str">
         <f>'Estimate (3)'!B58</f>
         <v>VAT calculation</v>
       </c>
@@ -4551,20 +4597,24 @@
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12">
-        <f>V!J66</f>
-        <v>103.52995110905256</v>
+        <f>V!J64</f>
+        <v>34.639407860372181</v>
       </c>
       <c r="J33" s="28">
         <f>I33-F33</f>
-        <v>5.6851857765315401</v>
+        <v>-63.20535747214884</v>
       </c>
       <c r="K33" s="14"/>
       <c r="M33" s="1">
         <f t="shared" si="0"/>
         <v>122.30595666565128</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N33" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="12"/>
@@ -4576,12 +4626,8 @@
       <c r="I34" s="12"/>
       <c r="J34" s="28"/>
       <c r="K34" s="14"/>
-      <c r="M34" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f>'Estimate (3)'!A60</f>
         <v>9</v>
@@ -4607,11 +4653,11 @@
         <v>102494.07193699971</v>
       </c>
       <c r="G35" s="12">
-        <f>V!G74</f>
+        <f>V!G72</f>
         <v>7.2088592413899129</v>
       </c>
       <c r="H35" s="12">
-        <f>V!I74</f>
+        <f>V!I72</f>
         <v>14362.76</v>
       </c>
       <c r="I35" s="12">
@@ -4627,10 +4673,14 @@
         <f t="shared" si="0"/>
         <v>128117.58992124963</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N35" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="32" t="str">
+      <c r="B36" s="100" t="str">
         <f>'Estimate (3)'!B67</f>
         <v>VAT calculation</v>
       </c>
@@ -4644,7 +4694,7 @@
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12">
-        <f>V!J75</f>
+        <f>V!J73</f>
         <v>9663.6646851953028</v>
       </c>
       <c r="J36" s="28">
@@ -4656,8 +4706,12 @@
         <f t="shared" si="0"/>
         <v>11957.658971554984</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="12"/>
@@ -4669,12 +4723,8 @@
       <c r="I37" s="12"/>
       <c r="J37" s="28"/>
       <c r="K37" s="14"/>
-      <c r="M37" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <f>'Estimate (3)'!A69</f>
         <v>10</v>
@@ -4700,11 +4750,11 @@
         <v>9329.4971045412967</v>
       </c>
       <c r="G38" s="12">
-        <f>V!G80</f>
+        <f>V!G78</f>
         <v>7.8599656583672295E-2</v>
       </c>
       <c r="H38" s="12">
-        <f>V!I80</f>
+        <f>V!I78</f>
         <v>131940</v>
       </c>
       <c r="I38" s="12">
@@ -4720,10 +4770,14 @@
         <f t="shared" si="0"/>
         <v>11661.871380676621</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N38" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
-      <c r="B39" s="32" t="str">
+      <c r="B39" s="100" t="str">
         <f>'Estimate (3)'!B73</f>
         <v>VAT calculation</v>
       </c>
@@ -4737,7 +4791,7 @@
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12">
-        <f>V!J81</f>
+        <f>V!J79</f>
         <v>1085.1468587941799</v>
       </c>
       <c r="J39" s="28">
@@ -4749,8 +4803,12 @@
         <f t="shared" si="0"/>
         <v>1220.2804023163669</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N39" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="12"/>
@@ -4762,12 +4820,8 @@
       <c r="I40" s="12"/>
       <c r="J40" s="28"/>
       <c r="K40" s="14"/>
-      <c r="M40" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:14" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="72">
         <f>'Estimate (3)'!A75</f>
         <v>11</v>
@@ -4793,11 +4847,11 @@
         <v>18239.27417994514</v>
       </c>
       <c r="G41" s="73">
-        <f>V!G87</f>
+        <f>V!G85</f>
         <v>54.480000000000004</v>
       </c>
       <c r="H41" s="73">
-        <f>V!I87</f>
+        <f>V!I85</f>
         <v>405.86</v>
       </c>
       <c r="I41" s="73">
@@ -4813,10 +4867,14 @@
         <f t="shared" si="0"/>
         <v>22799.092724931426</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N41" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
-      <c r="B42" s="32" t="str">
+      <c r="B42" s="100" t="str">
         <f>'Estimate (3)'!B79</f>
         <v>VAT calculation</v>
       </c>
@@ -4830,7 +4888,7 @@
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12">
-        <f>V!J88</f>
+        <f>V!J86</f>
         <v>790.83494880000012</v>
       </c>
       <c r="J42" s="74">
@@ -4842,8 +4900,12 @@
         <f t="shared" si="0"/>
         <v>815.43635229061283</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N42" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="12"/>
@@ -4855,12 +4917,8 @@
       <c r="I43" s="12"/>
       <c r="J43" s="28"/>
       <c r="K43" s="14"/>
-      <c r="M43" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <f>'Estimate (3)'!A81</f>
         <v>12</v>
@@ -4886,11 +4944,11 @@
         <v>500</v>
       </c>
       <c r="G44" s="12">
-        <f>V!C90</f>
+        <f>V!C88</f>
         <v>1</v>
       </c>
       <c r="H44" s="12">
-        <f>V!I90</f>
+        <f>V!I88</f>
         <v>500</v>
       </c>
       <c r="I44" s="12">
@@ -4906,8 +4964,12 @@
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N44" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="12"/>
@@ -4920,7 +4982,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="14"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6" t="s">
         <v>16</v>
@@ -4936,23 +4998,219 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7">
         <f>SUM(I13:I44)</f>
-        <v>570675.01263534476</v>
+        <v>564688.31314685999</v>
       </c>
       <c r="J46" s="13">
         <f>I46-F46</f>
-        <v>7040.0845652095741</v>
+        <v>1053.3850767248077</v>
       </c>
       <c r="K46" s="5"/>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="49" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B49" s="101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="103" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="101" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="104">
+        <f>1225/360*G13</f>
+        <v>70.723333333333343</v>
+      </c>
+      <c r="D50" s="105"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="106">
+        <f>19284/360*G13</f>
+        <v>1113.3296000000003</v>
+      </c>
+      <c r="D51" s="106">
+        <f>C51*0.13</f>
+        <v>144.73284800000005</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="107"/>
+      <c r="D52" s="107"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="107"/>
+      <c r="D53" s="107"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="107"/>
+      <c r="D54" s="107"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C55" s="107"/>
+      <c r="D55" s="107"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="107"/>
+      <c r="D57" s="107"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C58" s="107"/>
+      <c r="D58" s="107"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C59" s="107"/>
+      <c r="D59" s="107"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C60" s="107"/>
+      <c r="D60" s="107"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C61" s="107"/>
+      <c r="D61" s="107"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C62" s="107"/>
+      <c r="D62" s="107"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="107"/>
+      <c r="D63" s="107"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="107"/>
+      <c r="D64" s="107"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" s="107"/>
+      <c r="D65" s="107"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C66" s="107"/>
+      <c r="D66" s="107"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="107"/>
+      <c r="D67" s="107"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C68" s="107"/>
+      <c r="D68" s="107"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C69" s="107"/>
+      <c r="D69" s="107"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C70" s="107"/>
+      <c r="D70" s="107"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C71" s="107"/>
+      <c r="D71" s="107"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C72" s="107"/>
+      <c r="D72" s="107"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C73" s="107"/>
+      <c r="D73" s="107"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="107"/>
+      <c r="D74" s="107"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C75" s="107"/>
+      <c r="D75" s="107"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C76" s="107"/>
+      <c r="D76" s="107"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C77" s="107"/>
+      <c r="D77" s="107"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C78" s="107"/>
+      <c r="D78" s="107"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C79" s="107"/>
+      <c r="D79" s="107"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C80" s="107"/>
+      <c r="D80" s="107"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" s="107"/>
+      <c r="D81" s="107"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" s="107"/>
+      <c r="D83" s="107"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C84" s="107"/>
+      <c r="D84" s="107"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C85" s="107"/>
+      <c r="D85" s="107"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C86" s="107"/>
+      <c r="D86" s="107"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C87" s="107"/>
+      <c r="D87" s="107"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C88" s="107"/>
+      <c r="D88" s="107"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" s="107"/>
+      <c r="D89" s="107"/>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C90" s="107"/>
+      <c r="D90" s="107"/>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C91" s="107"/>
+      <c r="D91" s="107"/>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C92" s="107"/>
+      <c r="D92" s="107"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C93" s="107"/>
+      <c r="D93" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4966,6 +5224,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4981,10 +5246,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U156"/>
+  <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M64" sqref="M1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5001,119 +5266,116 @@
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="86" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="83" t="s">
+      <c r="H6" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="O6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="78" t="s">
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5147,11 +5409,8 @@
       <c r="K8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:14" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -5167,14 +5426,8 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
-      <c r="N9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="str">
         <f>B30</f>
@@ -5191,25 +5444,20 @@
         <v>1.6</v>
       </c>
       <c r="F10" s="38">
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="G10" s="39">
         <f>PRODUCT(C10:F10)</f>
-        <v>28.058400000000006</v>
+        <v>20.784000000000002</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="21"/>
       <c r="M10" s="25"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="25"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -5220,7 +5468,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="23">
         <f>SUM(G10:G10)</f>
-        <v>28.058400000000006</v>
+        <v>20.784000000000002</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>41</v>
@@ -5230,18 +5478,13 @@
       </c>
       <c r="J11" s="41">
         <f>G11*I11</f>
-        <v>1813.4143920000004</v>
+        <v>1343.26992</v>
       </c>
       <c r="K11" s="21"/>
       <c r="M11" s="25"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="25"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -5255,18 +5498,13 @@
       <c r="I12" s="23"/>
       <c r="J12" s="41">
         <f>0.13*G11*19284/360</f>
-        <v>195.38934480000006</v>
+        <v>144.73284800000002</v>
       </c>
       <c r="K12" s="21"/>
       <c r="M12" s="25"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="25"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -5279,14 +5517,9 @@
       <c r="J13" s="41"/>
       <c r="K13" s="21"/>
       <c r="M13" s="25"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-    </row>
-    <row r="14" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:14" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -5303,14 +5536,9 @@
       <c r="J14" s="41"/>
       <c r="K14" s="21"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="25"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>64</v>
@@ -5319,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="20">
-        <f>D69</f>
+        <f>D67</f>
         <v>20.95</v>
       </c>
       <c r="E15" s="21">
@@ -5337,7 +5565,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>42</v>
@@ -5362,7 +5590,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="19"/>
@@ -5375,7 +5603,7 @@
       <c r="J17" s="41"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:21" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -5392,7 +5620,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="37" t="s">
         <v>66</v>
@@ -5418,7 +5646,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37"/>
       <c r="C20" s="19">
@@ -5441,7 +5669,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -5466,7 +5694,7 @@
       </c>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="37"/>
       <c r="C22" s="19"/>
@@ -5479,7 +5707,7 @@
       <c r="J22" s="41"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -5496,7 +5724,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="37" t="str">
         <f>B15</f>
@@ -5506,24 +5734,23 @@
         <v>1</v>
       </c>
       <c r="D24" s="20">
-        <f>D69+D71</f>
+        <f>D67+D69</f>
         <v>22.11</v>
       </c>
       <c r="E24" s="21">
-        <f>E15</f>
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="39">
         <f>PRODUCT(C24:F24)</f>
-        <v>7.7384999999999993</v>
+        <v>5.0853000000000002</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="23"/>
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>80</v>
@@ -5548,7 +5775,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37" t="s">
         <v>42</v>
@@ -5559,7 +5786,7 @@
       <c r="F26" s="21"/>
       <c r="G26" s="23">
         <f>SUM(G24:G25)</f>
-        <v>9.3957691252666855</v>
+        <v>6.7425691252666873</v>
       </c>
       <c r="H26" s="22" t="s">
         <v>57</v>
@@ -5569,11 +5796,11 @@
       </c>
       <c r="J26" s="41">
         <f>G26*I26</f>
-        <v>9536.4237890719287</v>
+        <v>6843.5053850719296</v>
       </c>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="37" t="s">
         <v>40</v>
@@ -5587,11 +5814,11 @@
       <c r="I27" s="23"/>
       <c r="J27" s="41">
         <f>0.13*G26*8617.2/10</f>
-        <v>1052.5478821812251</v>
+        <v>755.32686666122538</v>
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="37"/>
       <c r="C28" s="19"/>
@@ -5604,7 +5831,7 @@
       <c r="J28" s="41"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>5</v>
       </c>
@@ -5620,19 +5847,12 @@
       <c r="I29" s="23"/>
       <c r="J29" s="41"/>
       <c r="K29" s="21"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="81"/>
-      <c r="S29" s="81"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="81"/>
-    </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="77"/>
+      <c r="N29" s="77"/>
+      <c r="O29" s="77"/>
+      <c r="P29" s="77"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="37" t="str">
         <f>B37</f>
@@ -5660,14 +5880,9 @@
       <c r="J30" s="40"/>
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="25"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37"/>
       <c r="C31" s="36">
@@ -5692,14 +5907,9 @@
       <c r="J31" s="40"/>
       <c r="K31" s="21"/>
       <c r="M31" s="25"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-    </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N31" s="25"/>
+    </row>
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="37"/>
       <c r="C32" s="36">
@@ -5724,14 +5934,9 @@
       <c r="J32" s="40"/>
       <c r="K32" s="21"/>
       <c r="M32" s="25"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-    </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N32" s="25"/>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>42</v>
@@ -5756,7 +5961,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37" t="s">
         <v>40</v>
@@ -5774,7 +5979,7 @@
       </c>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="37"/>
       <c r="C35" s="42"/>
@@ -5787,7 +5992,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -5804,14 +6009,9 @@
       <c r="J36" s="41"/>
       <c r="K36" s="21"/>
       <c r="M36" s="25"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-    </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="25"/>
+    </row>
+    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="37" t="s">
         <v>62</v>
@@ -5838,14 +6038,9 @@
       <c r="J37" s="40"/>
       <c r="K37" s="21"/>
       <c r="M37" s="25"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="25"/>
-    </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="25"/>
+    </row>
+    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="37"/>
       <c r="C38" s="36">
@@ -5870,14 +6065,9 @@
       <c r="J38" s="40"/>
       <c r="K38" s="21"/>
       <c r="M38" s="25"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N38" s="25"/>
+    </row>
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="37" t="s">
         <v>62</v>
@@ -5904,14 +6094,9 @@
       <c r="J39" s="40"/>
       <c r="K39" s="21"/>
       <c r="M39" s="25"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-    </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N39" s="25"/>
+    </row>
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="37"/>
       <c r="C40" s="36">
@@ -5936,14 +6121,9 @@
       <c r="J40" s="40"/>
       <c r="K40" s="21"/>
       <c r="M40" s="25"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N40" s="25"/>
+    </row>
+    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="37" t="s">
         <v>62</v>
@@ -5970,14 +6150,9 @@
       <c r="J41" s="40"/>
       <c r="K41" s="21"/>
       <c r="M41" s="25"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-    </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N41" s="25"/>
+    </row>
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="37"/>
       <c r="C42" s="36">
@@ -6002,14 +6177,9 @@
       <c r="J42" s="40"/>
       <c r="K42" s="21"/>
       <c r="M42" s="25"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="25"/>
-      <c r="S42" s="25"/>
-    </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N42" s="25"/>
+    </row>
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="37" t="s">
         <v>73</v>
@@ -6018,7 +6188,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="38">
-        <f>D69</f>
+        <f>D67</f>
         <v>20.95</v>
       </c>
       <c r="E43" s="38">
@@ -6037,14 +6207,9 @@
       <c r="J43" s="40"/>
       <c r="K43" s="21"/>
       <c r="M43" s="25"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-    </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N43" s="25"/>
+    </row>
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="37"/>
       <c r="C44" s="47">
@@ -6069,14 +6234,9 @@
       <c r="J44" s="40"/>
       <c r="K44" s="21"/>
       <c r="M44" s="25"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="25"/>
-      <c r="S44" s="25"/>
-    </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N44" s="25"/>
+    </row>
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="37"/>
       <c r="C45" s="47">
@@ -6101,14 +6261,9 @@
       <c r="J45" s="40"/>
       <c r="K45" s="21"/>
       <c r="M45" s="25"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-    </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N45" s="25"/>
+    </row>
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>80</v>
@@ -6136,14 +6291,9 @@
       <c r="J46" s="40"/>
       <c r="K46" s="21"/>
       <c r="M46" s="25"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
-    </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N46" s="25"/>
+    </row>
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="37"/>
       <c r="C47" s="47">
@@ -6168,14 +6318,9 @@
       <c r="J47" s="40"/>
       <c r="K47" s="21"/>
       <c r="M47" s="25"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="25"/>
-    </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N47" s="25"/>
+    </row>
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="37" t="s">
         <v>42</v>
@@ -6200,7 +6345,7 @@
       </c>
       <c r="K48" s="36"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="37" t="s">
         <v>40</v>
@@ -6218,7 +6363,7 @@
       </c>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="37"/>
       <c r="C50" s="42"/>
@@ -6231,7 +6376,7 @@
       <c r="J50" s="45"/>
       <c r="K50" s="36"/>
     </row>
-    <row r="51" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A51" s="63">
         <v>7</v>
       </c>
@@ -6248,7 +6393,7 @@
       <c r="J51" s="45"/>
       <c r="K51" s="29"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="37" t="s">
         <v>62</v>
@@ -6276,14 +6421,9 @@
       <c r="J52" s="40"/>
       <c r="K52" s="21"/>
       <c r="M52" s="25"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="25"/>
-    </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N52" s="25"/>
+    </row>
+    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="37"/>
       <c r="C53" s="36">
@@ -6309,14 +6449,9 @@
       <c r="J53" s="40"/>
       <c r="K53" s="21"/>
       <c r="M53" s="25"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="25"/>
-    </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N53" s="25"/>
+    </row>
+    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="37"/>
       <c r="C54" s="36">
@@ -6342,14 +6477,9 @@
       <c r="J54" s="40"/>
       <c r="K54" s="21"/>
       <c r="M54" s="25"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="25"/>
-    </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N54" s="25"/>
+    </row>
+    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="37" t="s">
         <v>42</v>
@@ -6374,7 +6504,7 @@
       </c>
       <c r="K55" s="36"/>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="37" t="s">
         <v>40</v>
@@ -6392,7 +6522,7 @@
       </c>
       <c r="K56" s="36"/>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="37"/>
       <c r="C57" s="42"/>
@@ -6405,7 +6535,7 @@
       <c r="J57" s="44"/>
       <c r="K57" s="36"/>
     </row>
-    <row r="58" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
         <v>8</v>
       </c>
@@ -6422,7 +6552,7 @@
       <c r="J58" s="41"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="37" t="s">
         <v>56</v>
@@ -6431,172 +6561,161 @@
         <v>1</v>
       </c>
       <c r="D59" s="38">
-        <f>(12.833+21+2+5.5+10.833+26.5)/3.281</f>
-        <v>23.976226760134104</v>
+        <f>(12.833-1.5+21-1.5+2-1.5+5.5-1.5+10.833-1.5+26.5-1.5+12.833-1.5-0.75-0.75)/3.281</f>
+        <v>24.230112770496799</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38">
-        <f>9/3.281</f>
-        <v>2.7430661383724475</v>
+        <f>8.5/3.281</f>
+        <v>2.5906735751295336</v>
       </c>
       <c r="G59" s="39">
-        <f t="shared" ref="G59:G63" si="6">PRODUCT(C59:F59)</f>
-        <v>65.7683757516632</v>
+        <f t="shared" ref="G59:G62" si="6">PRODUCT(C59:F59)</f>
+        <v>62.772312876934713</v>
       </c>
       <c r="H59" s="40"/>
       <c r="I59" s="40"/>
       <c r="J59" s="40"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="37"/>
+      <c r="B60" s="37" t="s">
+        <v>59</v>
+      </c>
       <c r="C60" s="36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D60" s="38">
-        <f>(12.833-1.5+21-1.5+2-1.5+5.5-1.5+10.833-1.5+26.5-1.5+12.833-1.5-0.75-0.75)/3.281</f>
-        <v>24.230112770496799</v>
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38">
-        <f>8.5/3.281</f>
-        <v>2.5906735751295336</v>
+        <f>7/3.281</f>
+        <v>2.1334958854007922</v>
       </c>
       <c r="G60" s="39">
         <f t="shared" si="6"/>
-        <v>62.772312876934713</v>
+        <v>-1.9507734398666188</v>
       </c>
       <c r="H60" s="40"/>
       <c r="I60" s="40"/>
       <c r="J60" s="40"/>
       <c r="K60" s="21"/>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
-      <c r="B61" s="37" t="s">
-        <v>59</v>
-      </c>
+      <c r="B61" s="37"/>
       <c r="C61" s="36">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="D61" s="38">
-        <f>3/3.281</f>
-        <v>0.91435537945748246</v>
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
       </c>
       <c r="E61" s="38"/>
       <c r="F61" s="38">
-        <f>7/3.281</f>
-        <v>2.1334958854007922</v>
+        <f>6/3.281</f>
+        <v>1.8287107589149649</v>
       </c>
       <c r="G61" s="39">
-        <f t="shared" si="6"/>
-        <v>-3.9015468797332375</v>
+        <f>PRODUCT(C61:F61)</f>
+        <v>-1.393409599904728</v>
       </c>
       <c r="H61" s="40"/>
       <c r="I61" s="40"/>
       <c r="J61" s="40"/>
       <c r="K61" s="21"/>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
-      <c r="B62" s="37"/>
+      <c r="B62" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C62" s="36">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="D62" s="38">
-        <f>2.5/3.281</f>
-        <v>0.76196281621456874</v>
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38">
-        <f>6/3.281</f>
-        <v>1.8287107589149649</v>
+        <f>4/3.281</f>
+        <v>1.2191405059433098</v>
       </c>
       <c r="G62" s="39">
         <f t="shared" si="6"/>
-        <v>-2.786819199809456</v>
+        <v>-1.3005156265777458</v>
       </c>
       <c r="H62" s="40"/>
       <c r="I62" s="40"/>
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C63" s="36">
-        <v>-2</v>
-      </c>
-      <c r="D63" s="38">
-        <f>3.5/3.281</f>
-        <v>1.0667479427003961</v>
-      </c>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38">
-        <f>4/3.281</f>
-        <v>1.2191405059433098</v>
-      </c>
-      <c r="G63" s="39">
-        <f t="shared" si="6"/>
-        <v>-2.6010312531554916</v>
-      </c>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
+        <v>42</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="23">
+        <f>SUM(G59:G62)</f>
+        <v>58.12761421058562</v>
+      </c>
+      <c r="H63" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63" s="23">
+        <v>20.82</v>
+      </c>
+      <c r="J63" s="41">
+        <f>G63*I63</f>
+        <v>1210.2169278643926</v>
+      </c>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="36">
-        <v>1</v>
-      </c>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39">
-        <f>G87</f>
-        <v>54.480000000000004</v>
-      </c>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="41">
+        <f>0.13*G63*458.4/100</f>
+        <v>34.639407860372181</v>
+      </c>
       <c r="K64" s="21"/>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
-      <c r="B65" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="B65" s="37"/>
       <c r="C65" s="19"/>
       <c r="D65" s="20"/>
       <c r="E65" s="21"/>
       <c r="F65" s="21"/>
-      <c r="G65" s="23">
-        <f>SUM(G59:G64)</f>
-        <v>173.73129129589972</v>
-      </c>
-      <c r="H65" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I65" s="23">
-        <v>20.82</v>
-      </c>
-      <c r="J65" s="41">
-        <f>G65*I65</f>
-        <v>3617.0854847806322</v>
-      </c>
+      <c r="G65" s="23"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="41"/>
       <c r="K65" s="21"/>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="37" t="s">
-        <v>40</v>
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A66" s="18">
+        <v>9</v>
+      </c>
+      <c r="B66" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="20"/>
@@ -6605,368 +6724,348 @@
       <c r="G66" s="23"/>
       <c r="H66" s="22"/>
       <c r="I66" s="23"/>
-      <c r="J66" s="41">
-        <f>0.13*G65*458.4/100</f>
-        <v>103.52995110905256</v>
-      </c>
+      <c r="J66" s="41"/>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="41"/>
+      <c r="B67" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="47">
+        <v>1</v>
+      </c>
+      <c r="D67" s="38">
+        <f>3.92+3.94+(3.52+3.49)+3.98+2.1</f>
+        <v>20.95</v>
+      </c>
+      <c r="E67" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="F67" s="38">
+        <f>1.47-0.23</f>
+        <v>1.24</v>
+      </c>
+      <c r="G67" s="39">
+        <f>PRODUCT(C67:F67)</f>
+        <v>5.9749400000000001</v>
+      </c>
+      <c r="H67" s="40"/>
+      <c r="I67" s="40"/>
+      <c r="J67" s="40"/>
       <c r="K67" s="21"/>
     </row>
-    <row r="68" spans="1:16" ht="30" x14ac:dyDescent="0.3">
-      <c r="A68" s="18">
-        <v>9</v>
-      </c>
-      <c r="B68" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="22"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="41"/>
+    <row r="68" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="18"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="47">
+        <v>1</v>
+      </c>
+      <c r="D68" s="38">
+        <f>3.94-0.9</f>
+        <v>3.04</v>
+      </c>
+      <c r="E68" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="F68" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G68" s="39">
+        <f>PRODUCT(C68:F68)</f>
+        <v>0.83904000000000001</v>
+      </c>
+      <c r="H68" s="40"/>
+      <c r="I68" s="40"/>
+      <c r="J68" s="40"/>
       <c r="K68" s="21"/>
-      <c r="N68">
-        <f>18.833*2</f>
-        <v>37.665999999999997</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="37" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C69" s="47">
         <v>1</v>
       </c>
       <c r="D69" s="38">
-        <f>3.92+3.94+(3.52+3.49)+3.98+2.1</f>
-        <v>20.95</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E69" s="38">
         <v>0.23</v>
       </c>
       <c r="F69" s="38">
-        <f>1.47-0.23</f>
-        <v>1.24</v>
+        <f>1.47-1.18-0.05-0.1</f>
+        <v>0.14000000000000004</v>
       </c>
       <c r="G69" s="39">
         <f>PRODUCT(C69:F69)</f>
-        <v>5.9749400000000001</v>
+        <v>3.735200000000001E-2</v>
       </c>
       <c r="H69" s="40"/>
       <c r="I69" s="40"/>
       <c r="J69" s="40"/>
       <c r="K69" s="21"/>
-      <c r="M69">
-        <f>19.083*2/3.281</f>
-        <v>11.632429137458091</v>
-      </c>
-      <c r="N69">
-        <f>18.833*2/3.281</f>
-        <v>11.480036574215177</v>
-      </c>
-      <c r="P69">
-        <f>0.75-0.075*2</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
-      <c r="B70" s="37"/>
+      <c r="B70" s="37" t="s">
+        <v>78</v>
+      </c>
       <c r="C70" s="47">
-        <v>1</v>
+        <f>0.5*7</f>
+        <v>3.5</v>
       </c>
       <c r="D70" s="38">
-        <f>3.94-0.9</f>
-        <v>3.04</v>
+        <f>2.42/3.281</f>
+        <v>0.73758000609570251</v>
       </c>
       <c r="E70" s="38">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="F70" s="38">
-        <v>1.2</v>
+        <f>7.5/12/3.281</f>
+        <v>0.19049070405364218</v>
       </c>
       <c r="G70" s="39">
         <f>PRODUCT(C70:F70)</f>
-        <v>0.83904000000000001</v>
+        <v>0.14752724138991305</v>
       </c>
       <c r="H70" s="40"/>
       <c r="I70" s="40"/>
       <c r="J70" s="40"/>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C71" s="47">
         <v>1</v>
       </c>
       <c r="D71" s="38">
-        <v>1.1599999999999999</v>
+        <v>3</v>
       </c>
       <c r="E71" s="38">
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="F71" s="38">
-        <f>1.47-1.18-0.05-0.1</f>
-        <v>0.14000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="G71" s="39">
         <f>PRODUCT(C71:F71)</f>
-        <v>3.735200000000001E-2</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="H71" s="40"/>
       <c r="I71" s="40"/>
       <c r="J71" s="40"/>
       <c r="K71" s="21"/>
     </row>
-    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C72" s="47">
-        <f>0.5*7</f>
-        <v>3.5</v>
-      </c>
-      <c r="D72" s="38">
-        <f>2.42/3.281</f>
-        <v>0.73758000609570251</v>
-      </c>
-      <c r="E72" s="38">
-        <v>0.3</v>
-      </c>
-      <c r="F72" s="38">
-        <f>7.5/12/3.281</f>
-        <v>0.19049070405364218</v>
-      </c>
-      <c r="G72" s="39">
-        <f>PRODUCT(C72:F72)</f>
-        <v>0.14752724138991305</v>
-      </c>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
-      <c r="J72" s="40"/>
+        <v>42</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="23">
+        <f>SUM(G67:G71)</f>
+        <v>7.2088592413899129</v>
+      </c>
+      <c r="H72" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="23">
+        <v>14362.76</v>
+      </c>
+      <c r="J72" s="41">
+        <f>G72*I72</f>
+        <v>103539.11515786538</v>
+      </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="47">
-        <v>1</v>
-      </c>
-      <c r="D73" s="38">
-        <v>3</v>
-      </c>
-      <c r="E73" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="F73" s="38">
-        <v>0.7</v>
-      </c>
-      <c r="G73" s="39">
-        <f>PRODUCT(C73:F73)</f>
-        <v>0.21000000000000002</v>
-      </c>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="41">
+        <f>0.13*G72*10311.74</f>
+        <v>9663.6646851953028</v>
+      </c>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
-      <c r="B74" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="B74" s="37"/>
       <c r="C74" s="19"/>
       <c r="D74" s="20"/>
       <c r="E74" s="21"/>
       <c r="F74" s="21"/>
-      <c r="G74" s="23">
-        <f>SUM(G69:G73)</f>
-        <v>7.2088592413899129</v>
-      </c>
-      <c r="H74" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I74" s="23">
-        <v>14362.76</v>
-      </c>
-      <c r="J74" s="41">
-        <f>G74*I74</f>
-        <v>103539.11515786538</v>
-      </c>
+      <c r="G74" s="23"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="41"/>
       <c r="K74" s="21"/>
     </row>
-    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="18"/>
-      <c r="B75" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75" s="19"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="23"/>
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A75" s="18">
+        <v>10</v>
+      </c>
+      <c r="B75" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="F75" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G75" s="68" t="s">
+        <v>70</v>
+      </c>
       <c r="H75" s="22"/>
       <c r="I75" s="23"/>
-      <c r="J75" s="41">
-        <f>0.13*G74*10311.74</f>
-        <v>9663.6646851953028</v>
-      </c>
+      <c r="J75" s="41"/>
       <c r="K75" s="21"/>
-      <c r="M75">
-        <f>14/3.281</f>
-        <v>4.2669917708015843</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="23"/>
+      <c r="B76" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" s="19">
+        <v>4</v>
+      </c>
+      <c r="D76" s="20">
+        <f>3.92+3.94+3.52+3.49+3.98+2.1</f>
+        <v>20.95</v>
+      </c>
+      <c r="E76" s="21">
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="F76" s="21">
+        <f>PRODUCT(C76:E76)</f>
+        <v>51.728395061728392</v>
+      </c>
+      <c r="G76" s="69">
+        <f>F76/1000</f>
+        <v>5.172839506172839E-2</v>
+      </c>
       <c r="H76" s="22"/>
       <c r="I76" s="23"/>
       <c r="J76" s="41"/>
       <c r="K76" s="21"/>
     </row>
-    <row r="77" spans="1:16" ht="30" x14ac:dyDescent="0.3">
-      <c r="A77" s="18">
-        <v>10</v>
-      </c>
-      <c r="B77" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="E77" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="F77" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G77" s="68" t="s">
-        <v>70</v>
+    <row r="77" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="18"/>
+      <c r="B77" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="19">
+        <f>2*TRUNC(D76/(8/12/3.281),0)</f>
+        <v>206</v>
+      </c>
+      <c r="D77" s="20">
+        <f>(7+3+3)/12/3.281</f>
+        <v>0.33018388702631307</v>
+      </c>
+      <c r="E77" s="21">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F77" s="21">
+        <f>PRODUCT(C77:E77)</f>
+        <v>26.871261521943897</v>
+      </c>
+      <c r="G77" s="69">
+        <f>F77/1000</f>
+        <v>2.6871261521943898E-2</v>
       </c>
       <c r="H77" s="22"/>
       <c r="I77" s="23"/>
       <c r="J77" s="41"/>
       <c r="K77" s="21"/>
     </row>
-    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="19">
-        <v>4</v>
-      </c>
-      <c r="D78" s="20">
-        <f>3.92+3.94+3.52+3.49+3.98+2.1</f>
-        <v>20.95</v>
-      </c>
-      <c r="E78" s="21">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
-      </c>
-      <c r="F78" s="21">
-        <f>PRODUCT(C78:E78)</f>
-        <v>51.728395061728392</v>
-      </c>
-      <c r="G78" s="69">
-        <f>F78/1000</f>
-        <v>5.172839506172839E-2</v>
-      </c>
-      <c r="H78" s="22"/>
-      <c r="I78" s="23"/>
-      <c r="J78" s="41"/>
+        <v>42</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="23">
+        <f>SUM(G76:G77)</f>
+        <v>7.8599656583672295E-2</v>
+      </c>
+      <c r="H78" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I78" s="23">
+        <v>131940</v>
+      </c>
+      <c r="J78" s="41">
+        <f>G78*I78</f>
+        <v>10370.438689649722</v>
+      </c>
       <c r="K78" s="21"/>
     </row>
-    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="19">
-        <f>2*TRUNC(D78/(8/12/3.281),0)</f>
-        <v>206</v>
-      </c>
-      <c r="D79" s="20">
-        <f>(7+3+3)/12/3.281</f>
-        <v>0.33018388702631307</v>
-      </c>
-      <c r="E79" s="21">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F79" s="21">
-        <f>PRODUCT(C79:E79)</f>
-        <v>26.871261521943897</v>
-      </c>
-      <c r="G79" s="69">
-        <f>F79/1000</f>
-        <v>2.6871261521943898E-2</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="23"/>
       <c r="H79" s="22"/>
       <c r="I79" s="23"/>
-      <c r="J79" s="41"/>
+      <c r="J79" s="41">
+        <f>0.13*G78*106200</f>
+        <v>1085.1468587941799</v>
+      </c>
       <c r="K79" s="21"/>
     </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
-      <c r="B80" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="B80" s="37"/>
       <c r="C80" s="19"/>
       <c r="D80" s="20"/>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
-      <c r="G80" s="23">
-        <f>SUM(G78:G79)</f>
-        <v>7.8599656583672295E-2</v>
-      </c>
-      <c r="H80" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I80" s="23">
-        <v>131940</v>
-      </c>
-      <c r="J80" s="41">
-        <f>G80*I80</f>
-        <v>10370.438689649722</v>
-      </c>
+      <c r="G80" s="23"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="41"/>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="37" t="s">
-        <v>40</v>
+    <row r="81" spans="1:14" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="18">
+        <v>11</v>
+      </c>
+      <c r="B81" s="70" t="s">
+        <v>74</v>
       </c>
       <c r="C81" s="19"/>
       <c r="D81" s="20"/>
@@ -6975,162 +7074,173 @@
       <c r="G81" s="23"/>
       <c r="H81" s="22"/>
       <c r="I81" s="23"/>
-      <c r="J81" s="41">
-        <f>0.13*G80*106200</f>
-        <v>1085.1468587941799</v>
-      </c>
+      <c r="J81" s="41"/>
       <c r="K81" s="21"/>
     </row>
-    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="41"/>
+      <c r="B82" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="36">
+        <v>1</v>
+      </c>
+      <c r="D82" s="38">
+        <f>3.92+3.94+0.23+0.23+3.52+3.49+3.98+0.23+0.23+2.1</f>
+        <v>21.87</v>
+      </c>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G82" s="39">
+        <f t="shared" ref="G82:G84" si="7">PRODUCT(C82:F82)</f>
+        <v>26.244</v>
+      </c>
+      <c r="H82" s="40"/>
+      <c r="I82" s="40"/>
+      <c r="J82" s="40"/>
       <c r="K82" s="21"/>
     </row>
-    <row r="83" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="18">
-        <v>11</v>
-      </c>
-      <c r="B83" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="22"/>
-      <c r="I83" s="23"/>
-      <c r="J83" s="41"/>
+    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="18"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="36">
+        <v>1</v>
+      </c>
+      <c r="D83" s="38">
+        <f>3.92-0.23+3.94+3.52+3.49-0.23-0.23+3.98+2.1-0.23</f>
+        <v>20.03</v>
+      </c>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="G83" s="39">
+        <f t="shared" si="7"/>
+        <v>24.036000000000001</v>
+      </c>
+      <c r="H83" s="40"/>
+      <c r="I83" s="40"/>
+      <c r="J83" s="40"/>
       <c r="K83" s="21"/>
     </row>
-    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="18"/>
       <c r="B84" s="37" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C84" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84" s="38">
-        <f>3.92+3.94+0.23+0.23+3.52+3.49+3.98+0.23+0.23+2.1</f>
-        <v>21.87</v>
+        <f>D71</f>
+        <v>3</v>
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38">
-        <v>1.2</v>
+        <f>F71</f>
+        <v>0.7</v>
       </c>
       <c r="G84" s="39">
-        <f t="shared" ref="G84:G86" si="7">PRODUCT(C84:F84)</f>
-        <v>26.244</v>
+        <f t="shared" si="7"/>
+        <v>4.1999999999999993</v>
       </c>
       <c r="H84" s="40"/>
       <c r="I84" s="40"/>
       <c r="J84" s="40"/>
       <c r="K84" s="21"/>
     </row>
-    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="36">
-        <v>1</v>
-      </c>
-      <c r="D85" s="38">
-        <f>3.92-0.23+3.94+3.52+3.49-0.23-0.23+3.98+2.1-0.23</f>
-        <v>20.03</v>
-      </c>
-      <c r="E85" s="38"/>
-      <c r="F85" s="38">
-        <v>1.2</v>
-      </c>
-      <c r="G85" s="39">
-        <f t="shared" si="7"/>
-        <v>24.036000000000001</v>
-      </c>
-      <c r="H85" s="40"/>
-      <c r="I85" s="40"/>
-      <c r="J85" s="40"/>
+      <c r="B85" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="23">
+        <f>SUM(G82:G84)</f>
+        <v>54.480000000000004</v>
+      </c>
+      <c r="H85" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I85" s="23">
+        <v>405.86</v>
+      </c>
+      <c r="J85" s="41">
+        <f>G85*I85</f>
+        <v>22111.252800000002</v>
+      </c>
       <c r="K85" s="21"/>
     </row>
-    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18"/>
       <c r="B86" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="36">
-        <v>2</v>
-      </c>
-      <c r="D86" s="38">
-        <f>D73</f>
-        <v>3</v>
-      </c>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38">
-        <f>F73</f>
-        <v>0.7</v>
-      </c>
-      <c r="G86" s="39">
-        <f t="shared" si="7"/>
-        <v>4.1999999999999993</v>
-      </c>
-      <c r="H86" s="40"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="C86" s="19"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="41">
+        <f>0.13*G85*11166.2/100</f>
+        <v>790.83494880000012</v>
+      </c>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18"/>
-      <c r="B87" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="B87" s="37"/>
       <c r="C87" s="19"/>
       <c r="D87" s="20"/>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
-      <c r="G87" s="23">
-        <f>SUM(G84:G86)</f>
-        <v>54.480000000000004</v>
-      </c>
-      <c r="H87" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="I87" s="23">
-        <v>405.86</v>
-      </c>
-      <c r="J87" s="41">
-        <f>G87*I87</f>
-        <v>22111.252800000002</v>
-      </c>
+      <c r="G87" s="23"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="23"/>
+      <c r="J87" s="41"/>
       <c r="K87" s="21"/>
     </row>
-    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="18"/>
-      <c r="B88" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C88" s="19"/>
+    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="18">
+        <v>12</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" s="19">
+        <v>1</v>
+      </c>
       <c r="D88" s="20"/>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
-      <c r="G88" s="23"/>
-      <c r="H88" s="22"/>
-      <c r="I88" s="23"/>
-      <c r="J88" s="41">
-        <f>0.13*G87*11166.2/100</f>
-        <v>790.83494880000012</v>
+      <c r="G88" s="34">
+        <f t="shared" ref="G88" si="8">PRODUCT(C88:F88)</f>
+        <v>1</v>
+      </c>
+      <c r="H88" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I88" s="23">
+        <v>500</v>
+      </c>
+      <c r="J88" s="34">
+        <f>G88*I88</f>
+        <v>500</v>
       </c>
       <c r="K88" s="21"/>
-    </row>
-    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M88" s="25"/>
+      <c r="N88" s="25"/>
+    </row>
+    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="18"/>
-      <c r="B89" s="37"/>
+      <c r="B89" s="24"/>
       <c r="C89" s="19"/>
       <c r="D89" s="20"/>
       <c r="E89" s="21"/>
@@ -7140,127 +7250,112 @@
       <c r="I89" s="23"/>
       <c r="J89" s="41"/>
       <c r="K89" s="21"/>
-    </row>
-    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="18">
-        <v>12</v>
-      </c>
-      <c r="B90" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="19">
-        <v>1</v>
-      </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="34">
-        <f t="shared" ref="G90" si="8">PRODUCT(C90:F90)</f>
-        <v>1</v>
-      </c>
-      <c r="H90" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I90" s="23">
-        <v>500</v>
-      </c>
-      <c r="J90" s="34">
-        <f>G90*I90</f>
-        <v>500</v>
-      </c>
-      <c r="K90" s="21"/>
-      <c r="M90" s="25"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
-      <c r="R90" s="25"/>
-      <c r="S90" s="25"/>
-    </row>
-    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="18"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="23"/>
-      <c r="H91" s="22"/>
-      <c r="I91" s="23"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="21"/>
-      <c r="M91" s="25"/>
-      <c r="N91" s="1">
-        <f>2.4*3.281</f>
-        <v>7.8743999999999996</v>
-      </c>
-      <c r="O91" s="1"/>
-      <c r="P91" s="1"/>
-      <c r="Q91" s="1"/>
-      <c r="R91" s="25"/>
-      <c r="S91" s="25"/>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A92" s="40"/>
-      <c r="B92" s="46" t="s">
+      <c r="M89" s="25"/>
+      <c r="N89" s="25"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A90" s="40"/>
+      <c r="B90" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C92" s="47"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="41"/>
-      <c r="H92" s="41"/>
-      <c r="I92" s="41"/>
-      <c r="J92" s="41">
-        <f>SUM(J10:J90)</f>
-        <v>570675.01263534476</v>
-      </c>
-      <c r="K92" s="36"/>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A93" s="58"/>
-      <c r="B93" s="61"/>
-      <c r="C93" s="62"/>
-      <c r="D93" s="59"/>
-      <c r="E93" s="59"/>
-      <c r="F93" s="59"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="60"/>
-      <c r="I93" s="60"/>
-      <c r="J93" s="60"/>
-      <c r="K93" s="57"/>
-    </row>
-    <row r="94" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="50"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="41"/>
+      <c r="H90" s="41"/>
+      <c r="I90" s="41"/>
+      <c r="J90" s="41">
+        <f>SUM(J10:J88)</f>
+        <v>564688.31314685999</v>
+      </c>
+      <c r="K90" s="36"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A91" s="58"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="62"/>
+      <c r="D91" s="59"/>
+      <c r="E91" s="59"/>
+      <c r="F91" s="59"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="60"/>
+      <c r="I91" s="60"/>
+      <c r="J91" s="60"/>
+      <c r="K91" s="57"/>
+    </row>
+    <row r="92" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="50"/>
+      <c r="B92" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" s="84">
+        <f>J90</f>
+        <v>564688.31314685999</v>
+      </c>
+      <c r="D92" s="84"/>
+      <c r="E92" s="39">
+        <v>100</v>
+      </c>
+      <c r="F92" s="51"/>
+      <c r="G92" s="52"/>
+      <c r="H92" s="51"/>
+      <c r="I92" s="53"/>
+      <c r="J92" s="54"/>
+      <c r="K92" s="55"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A93" s="56"/>
+      <c r="B93" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="87">
+        <v>500000</v>
+      </c>
+      <c r="D93" s="87"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="48"/>
+      <c r="H93" s="48"/>
+      <c r="I93" s="48"/>
+      <c r="J93" s="48"/>
+      <c r="K93" s="49"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A94" s="56"/>
       <c r="B94" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C94" s="77">
-        <f>J92</f>
-        <v>570675.01263534476</v>
-      </c>
-      <c r="D94" s="77"/>
+        <v>33</v>
+      </c>
+      <c r="C94" s="87">
+        <f>C93-C96-C97</f>
+        <v>475000</v>
+      </c>
+      <c r="D94" s="87"/>
       <c r="E94" s="39">
-        <v>100</v>
-      </c>
-      <c r="F94" s="51"/>
-      <c r="G94" s="52"/>
-      <c r="H94" s="51"/>
-      <c r="I94" s="53"/>
-      <c r="J94" s="54"/>
-      <c r="K94" s="55"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+        <f>C94/C92*100</f>
+        <v>84.117200399092638</v>
+      </c>
+      <c r="F94" s="49"/>
+      <c r="G94" s="48"/>
+      <c r="H94" s="48"/>
+      <c r="I94" s="48"/>
+      <c r="J94" s="48"/>
+      <c r="K94" s="49"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="56"/>
       <c r="B95" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C95" s="80">
-        <v>500000</v>
-      </c>
-      <c r="D95" s="80"/>
-      <c r="E95" s="39"/>
+        <v>34</v>
+      </c>
+      <c r="C95" s="84">
+        <f>C92-C94</f>
+        <v>89688.31314685999</v>
+      </c>
+      <c r="D95" s="84"/>
+      <c r="E95" s="39">
+        <f>100-E94</f>
+        <v>15.882799600907362</v>
+      </c>
       <c r="F95" s="49"/>
       <c r="G95" s="48"/>
       <c r="H95" s="48"/>
@@ -7268,19 +7363,18 @@
       <c r="J95" s="48"/>
       <c r="K95" s="49"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="56"/>
       <c r="B96" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C96" s="80">
-        <f>C95-C98-C99</f>
-        <v>475000</v>
-      </c>
-      <c r="D96" s="80"/>
+        <v>35</v>
+      </c>
+      <c r="C96" s="84">
+        <f>C93*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D96" s="84"/>
       <c r="E96" s="39">
-        <f>C96/C94*100</f>
-        <v>83.234764004556112</v>
+        <v>3</v>
       </c>
       <c r="F96" s="49"/>
       <c r="G96" s="48"/>
@@ -7292,16 +7386,15 @@
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="56"/>
       <c r="B97" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C97" s="77">
-        <f>C94-C96</f>
-        <v>95675.012635344756</v>
-      </c>
-      <c r="D97" s="77"/>
+        <v>36</v>
+      </c>
+      <c r="C97" s="84">
+        <f>C93*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D97" s="84"/>
       <c r="E97" s="39">
-        <f>100-E96</f>
-        <v>16.765235995443888</v>
+        <v>2</v>
       </c>
       <c r="F97" s="49"/>
       <c r="G97" s="48"/>
@@ -7310,59 +7403,21 @@
       <c r="J97" s="48"/>
       <c r="K97" s="49"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A98" s="56"/>
-      <c r="B98" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C98" s="77">
-        <f>C95*0.03</f>
-        <v>15000</v>
-      </c>
-      <c r="D98" s="77"/>
-      <c r="E98" s="39">
-        <v>3</v>
-      </c>
-      <c r="F98" s="49"/>
-      <c r="G98" s="48"/>
-      <c r="H98" s="48"/>
-      <c r="I98" s="48"/>
-      <c r="J98" s="48"/>
-      <c r="K98" s="49"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="56"/>
-      <c r="B99" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C99" s="77">
-        <f>C95*0.02</f>
-        <v>10000</v>
-      </c>
-      <c r="D99" s="77"/>
-      <c r="E99" s="39">
-        <v>2</v>
-      </c>
-      <c r="F99" s="49"/>
-      <c r="G99" s="48"/>
-      <c r="H99" s="48"/>
-      <c r="I99" s="48"/>
-      <c r="J99" s="48"/>
-      <c r="K99" s="49"/>
-    </row>
-    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="57"/>
-      <c r="B100" s="57"/>
-      <c r="C100" s="57"/>
-      <c r="D100" s="57"/>
-      <c r="E100" s="57"/>
-      <c r="F100" s="57"/>
-      <c r="G100" s="57"/>
-      <c r="H100" s="57"/>
-      <c r="I100" s="57"/>
-      <c r="J100" s="57"/>
-      <c r="K100" s="57"/>
-    </row>
+    <row r="98" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="57"/>
+      <c r="B98" s="57"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
+      <c r="F98" s="57"/>
+      <c r="G98" s="57"/>
+      <c r="H98" s="57"/>
+      <c r="I98" s="57"/>
+      <c r="J98" s="57"/>
+      <c r="K98" s="57"/>
+    </row>
+    <row r="99" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="101" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="102" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -7417,14 +7472,17 @@
     <row r="152" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="153" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="155" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="156" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="O29:U29"/>
-    <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -7432,11 +7490,6 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
estimate of chinimaya mam, sanagaun dhal byabasthapan, ukhutaar bhitri private baato, ganapati dhikurepati, paropakar valuation done along with site plan of gai goth
</commit_message>
<xml_diff>
--- a/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
+++ b/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="92">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -422,6 +422,15 @@
   </si>
   <si>
     <t>Skilled</t>
+  </si>
+  <si>
+    <t>unskilled</t>
+  </si>
+  <si>
+    <t>Brick</t>
+  </si>
+  <si>
+    <t>sand</t>
   </si>
 </sst>
 </file>
@@ -811,27 +820,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,6 +852,48 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,49 +909,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1537,116 +1546,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
       <c r="O6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="86" t="s">
+      <c r="H7" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2184,15 +2193,15 @@
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="77" t="s">
+      <c r="O30" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="77"/>
-      <c r="T30" s="77"/>
-      <c r="U30" s="77"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
@@ -3483,11 +3492,11 @@
       <c r="B85" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C85" s="84">
+      <c r="C85" s="85">
         <f>J83</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D85" s="84"/>
+      <c r="D85" s="85"/>
       <c r="E85" s="39">
         <v>100</v>
       </c>
@@ -3503,10 +3512,10 @@
       <c r="B86" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="87">
+      <c r="C86" s="88">
         <v>500000</v>
       </c>
-      <c r="D86" s="87"/>
+      <c r="D86" s="88"/>
       <c r="E86" s="39"/>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -3520,11 +3529,11 @@
       <c r="B87" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="87">
+      <c r="C87" s="88">
         <f>C86-C89-C90</f>
         <v>475000</v>
       </c>
-      <c r="D87" s="87"/>
+      <c r="D87" s="88"/>
       <c r="E87" s="39">
         <f>C87/C85*100</f>
         <v>84.274408192973809</v>
@@ -3541,11 +3550,11 @@
       <c r="B88" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C88" s="84">
+      <c r="C88" s="85">
         <f>C85-C87</f>
         <v>88634.928070135182</v>
       </c>
-      <c r="D88" s="84"/>
+      <c r="D88" s="85"/>
       <c r="E88" s="39">
         <f>100-E87</f>
         <v>15.725591807026191</v>
@@ -3562,11 +3571,11 @@
       <c r="B89" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="84">
+      <c r="C89" s="85">
         <f>C86*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D89" s="84"/>
+      <c r="D89" s="85"/>
       <c r="E89" s="39">
         <v>3</v>
       </c>
@@ -3582,11 +3591,11 @@
       <c r="B90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="84">
+      <c r="C90" s="85">
         <f>C86*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D90" s="84"/>
+      <c r="D90" s="85"/>
       <c r="E90" s="39">
         <v>2</v>
       </c>
@@ -3668,6 +3677,14 @@
     <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O30:U30"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="A7:F7"/>
@@ -3676,14 +3693,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="O30:U30"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -3696,10 +3705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3718,90 +3727,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
     </row>
     <row r="2" spans="1:14" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="88">
+      <c r="C6" s="103">
         <f>F46</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3809,11 +3818,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="88">
+      <c r="J6" s="103">
         <f>I46</f>
         <v>564688.31314685999</v>
       </c>
-      <c r="K6" s="89"/>
+      <c r="K6" s="104"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -3822,77 +3831,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="I7" s="96" t="s">
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="I7" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
     </row>
     <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="78" t="e">
+      <c r="A8" s="90" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="I8" s="97" t="s">
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="I8" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="98" t="e">
+      <c r="A9" s="101" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="I9" s="97" t="s">
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="I9" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="97"/>
-      <c r="K9" s="97"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99" t="s">
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="93" t="s">
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="94" t="s">
+      <c r="K11" s="97" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="93"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3911,8 +3920,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="93"/>
-      <c r="K12" s="94"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="97"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
@@ -3967,7 +3976,7 @@
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
-      <c r="B14" s="100" t="str">
+      <c r="B14" s="77" t="str">
         <f>'Estimate (3)'!B12</f>
         <v>VAT calculation</v>
       </c>
@@ -4195,7 +4204,7 @@
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
-      <c r="B21" s="100" t="str">
+      <c r="B21" s="77" t="str">
         <f>'Estimate (3)'!B28</f>
         <v>VAT calculation</v>
       </c>
@@ -4292,7 +4301,7 @@
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
-      <c r="B24" s="100" t="str">
+      <c r="B24" s="77" t="str">
         <f>'Estimate (3)'!B33</f>
         <v>VAT calculation</v>
       </c>
@@ -4389,7 +4398,7 @@
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
-      <c r="B27" s="100" t="str">
+      <c r="B27" s="77" t="str">
         <f>'Estimate (3)'!B43</f>
         <v>VAT calculation</v>
       </c>
@@ -4486,7 +4495,7 @@
     </row>
     <row r="30" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
-      <c r="B30" s="100" t="str">
+      <c r="B30" s="77" t="str">
         <f>'Estimate (3)'!B48</f>
         <v>VAT calculation</v>
       </c>
@@ -4583,7 +4592,7 @@
     </row>
     <row r="33" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
-      <c r="B33" s="100" t="str">
+      <c r="B33" s="77" t="str">
         <f>'Estimate (3)'!B58</f>
         <v>VAT calculation</v>
       </c>
@@ -4680,7 +4689,7 @@
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="100" t="str">
+      <c r="B36" s="77" t="str">
         <f>'Estimate (3)'!B67</f>
         <v>VAT calculation</v>
       </c>
@@ -4777,7 +4786,7 @@
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
-      <c r="B39" s="100" t="str">
+      <c r="B39" s="77" t="str">
         <f>'Estimate (3)'!B73</f>
         <v>VAT calculation</v>
       </c>
@@ -4874,7 +4883,7 @@
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
-      <c r="B42" s="100" t="str">
+      <c r="B42" s="77" t="str">
         <f>'Estimate (3)'!B79</f>
         <v>VAT calculation</v>
       </c>
@@ -5008,209 +5017,244 @@
       <c r="N46" s="1"/>
     </row>
     <row r="49" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B49" s="101" t="s">
+      <c r="B49" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="103" t="s">
+      <c r="C49" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="D49" s="101" t="s">
+      <c r="D49" s="78" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="101" t="s">
+      <c r="B50" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="104">
-        <f>1225/360*G13</f>
-        <v>70.723333333333343</v>
-      </c>
-      <c r="D50" s="105"/>
+      <c r="C50" s="81">
+        <f>(1225/360*G13)+(612.5/10*G20)</f>
+        <v>483.70569225591794</v>
+      </c>
+      <c r="D50" s="82"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="81">
+        <f>(2760/360*G13)+(G16*H16)+(G18*H18)+(920/10*G20)</f>
+        <v>2054.7098388028799</v>
+      </c>
+      <c r="D51" s="82"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="106">
+      <c r="C52" s="83">
         <f>19284/360*G13</f>
         <v>1113.3296000000003</v>
       </c>
-      <c r="D51" s="106">
-        <f>C51*0.13</f>
+      <c r="D52" s="83">
+        <f>C52*0.13</f>
         <v>144.73284800000005</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C52" s="107"/>
-      <c r="D52" s="107"/>
-    </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C53" s="107"/>
-      <c r="D53" s="107"/>
+      <c r="B53" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="84">
+        <f>(6360.9/10*G20)</f>
+        <v>4288.8807948908861</v>
+      </c>
+      <c r="D53" s="83">
+        <f t="shared" ref="D53:D54" si="2">C53*0.13</f>
+        <v>557.55450333581518</v>
+      </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
+      <c r="B54" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="84">
+        <f>(2256.3/10*G20)</f>
+        <v>1521.3258717339229</v>
+      </c>
+      <c r="D54" s="83">
+        <f t="shared" si="2"/>
+        <v>197.77236332540997</v>
+      </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C55" s="107"/>
-      <c r="D55" s="107"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C56" s="107"/>
-      <c r="D56" s="107"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="84"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C57" s="107"/>
-      <c r="D57" s="107"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="84"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C58" s="107"/>
-      <c r="D58" s="107"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="84"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C59" s="107"/>
-      <c r="D59" s="107"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="84"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C60" s="107"/>
-      <c r="D60" s="107"/>
+      <c r="C60" s="84"/>
+      <c r="D60" s="84"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C61" s="107"/>
-      <c r="D61" s="107"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="84"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C62" s="107"/>
-      <c r="D62" s="107"/>
+      <c r="C62" s="84"/>
+      <c r="D62" s="84"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C63" s="107"/>
-      <c r="D63" s="107"/>
+      <c r="C63" s="84"/>
+      <c r="D63" s="84"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C64" s="107"/>
-      <c r="D64" s="107"/>
+      <c r="C64" s="84"/>
+      <c r="D64" s="84"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C65" s="107"/>
-      <c r="D65" s="107"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C66" s="107"/>
-      <c r="D66" s="107"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="84"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C67" s="107"/>
-      <c r="D67" s="107"/>
+      <c r="C67" s="84"/>
+      <c r="D67" s="84"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C68" s="107"/>
-      <c r="D68" s="107"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="84"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C69" s="107"/>
-      <c r="D69" s="107"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C70" s="107"/>
-      <c r="D70" s="107"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C71" s="107"/>
-      <c r="D71" s="107"/>
+      <c r="C71" s="84"/>
+      <c r="D71" s="84"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C72" s="107"/>
-      <c r="D72" s="107"/>
+      <c r="C72" s="84"/>
+      <c r="D72" s="84"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C73" s="107"/>
-      <c r="D73" s="107"/>
+      <c r="C73" s="84"/>
+      <c r="D73" s="84"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C74" s="107"/>
-      <c r="D74" s="107"/>
+      <c r="C74" s="84"/>
+      <c r="D74" s="84"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C75" s="107"/>
-      <c r="D75" s="107"/>
+      <c r="C75" s="84"/>
+      <c r="D75" s="84"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C76" s="107"/>
-      <c r="D76" s="107"/>
+      <c r="C76" s="84"/>
+      <c r="D76" s="84"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C77" s="107"/>
-      <c r="D77" s="107"/>
+      <c r="C77" s="84"/>
+      <c r="D77" s="84"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C78" s="107"/>
-      <c r="D78" s="107"/>
+      <c r="C78" s="84"/>
+      <c r="D78" s="84"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C79" s="107"/>
-      <c r="D79" s="107"/>
+      <c r="C79" s="84"/>
+      <c r="D79" s="84"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C80" s="107"/>
-      <c r="D80" s="107"/>
+      <c r="C80" s="84"/>
+      <c r="D80" s="84"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C81" s="107"/>
-      <c r="D81" s="107"/>
+      <c r="C81" s="84"/>
+      <c r="D81" s="84"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C82" s="107"/>
-      <c r="D82" s="107"/>
+      <c r="C82" s="84"/>
+      <c r="D82" s="84"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C83" s="107"/>
-      <c r="D83" s="107"/>
+      <c r="C83" s="84"/>
+      <c r="D83" s="84"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C84" s="107"/>
-      <c r="D84" s="107"/>
+      <c r="C84" s="84"/>
+      <c r="D84" s="84"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C85" s="107"/>
-      <c r="D85" s="107"/>
+      <c r="C85" s="84"/>
+      <c r="D85" s="84"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C86" s="107"/>
-      <c r="D86" s="107"/>
+      <c r="C86" s="84"/>
+      <c r="D86" s="84"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C87" s="107"/>
-      <c r="D87" s="107"/>
+      <c r="C87" s="84"/>
+      <c r="D87" s="84"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C88" s="107"/>
-      <c r="D88" s="107"/>
+      <c r="C88" s="84"/>
+      <c r="D88" s="84"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C89" s="107"/>
-      <c r="D89" s="107"/>
+      <c r="C89" s="84"/>
+      <c r="D89" s="84"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C90" s="107"/>
-      <c r="D90" s="107"/>
+      <c r="C90" s="84"/>
+      <c r="D90" s="84"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C91" s="107"/>
-      <c r="D91" s="107"/>
+      <c r="C91" s="84"/>
+      <c r="D91" s="84"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C92" s="107"/>
-      <c r="D92" s="107"/>
+      <c r="C92" s="84"/>
+      <c r="D92" s="84"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C93" s="107"/>
-      <c r="D93" s="107"/>
+      <c r="C93" s="84"/>
+      <c r="D93" s="84"/>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C94" s="84"/>
+      <c r="D94" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -5224,13 +5268,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5267,113 +5304,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
     </row>
     <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="86" t="s">
+      <c r="H7" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -5847,10 +5884,10 @@
       <c r="I29" s="23"/>
       <c r="J29" s="41"/>
       <c r="K29" s="21"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="77"/>
-      <c r="P29" s="77"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="89"/>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
@@ -7289,11 +7326,11 @@
       <c r="B92" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="84">
+      <c r="C92" s="85">
         <f>J90</f>
         <v>564688.31314685999</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="85"/>
       <c r="E92" s="39">
         <v>100</v>
       </c>
@@ -7309,10 +7346,10 @@
       <c r="B93" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C93" s="87">
+      <c r="C93" s="88">
         <v>500000</v>
       </c>
-      <c r="D93" s="87"/>
+      <c r="D93" s="88"/>
       <c r="E93" s="39"/>
       <c r="F93" s="49"/>
       <c r="G93" s="48"/>
@@ -7326,11 +7363,11 @@
       <c r="B94" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C94" s="87">
+      <c r="C94" s="88">
         <f>C93-C96-C97</f>
         <v>475000</v>
       </c>
-      <c r="D94" s="87"/>
+      <c r="D94" s="88"/>
       <c r="E94" s="39">
         <f>C94/C92*100</f>
         <v>84.117200399092638</v>
@@ -7347,11 +7384,11 @@
       <c r="B95" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C95" s="84">
+      <c r="C95" s="85">
         <f>C92-C94</f>
         <v>89688.31314685999</v>
       </c>
-      <c r="D95" s="84"/>
+      <c r="D95" s="85"/>
       <c r="E95" s="39">
         <f>100-E94</f>
         <v>15.882799600907362</v>
@@ -7368,11 +7405,11 @@
       <c r="B96" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C96" s="84">
+      <c r="C96" s="85">
         <f>C93*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D96" s="84"/>
+      <c r="D96" s="85"/>
       <c r="E96" s="39">
         <v>3</v>
       </c>
@@ -7388,11 +7425,11 @@
       <c r="B97" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C97" s="84">
+      <c r="C97" s="85">
         <f>C93*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D97" s="84"/>
+      <c r="D97" s="85"/>
       <c r="E97" s="39">
         <v>2</v>
       </c>
@@ -7474,11 +7511,6 @@
     <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
     <mergeCell ref="M29:P29"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="C93:D93"/>
@@ -7490,6 +7522,11 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
VAT details of paropakar and ganapati dhikurepati complete
</commit_message>
<xml_diff>
--- a/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
+++ b/ofc/estimates/गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक/V गणपति ढिकुरेपाटी संरक्षण.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\गणपति ढिकुरेपाटी संरक्षण तथा ढिकुरेपाटी माझ गाँउ सडक\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate (3)" sheetId="19" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="101">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -452,16 +452,22 @@
   </si>
   <si>
     <t xml:space="preserve">गम </t>
+  </si>
+  <si>
+    <t>rod</t>
+  </si>
+  <si>
+    <t>wire binding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -665,7 +671,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -675,7 +681,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,14 +701,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,7 +717,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -736,7 +742,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,7 +772,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,7 +781,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -790,7 +796,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -806,11 +812,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,7 +831,7 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,7 +842,7 @@
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -857,15 +863,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,6 +887,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -908,24 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1549,133 +1555,133 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="93" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
       <c r="O6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="str">
         <f>B31</f>
@@ -1772,7 +1778,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -1804,7 +1810,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -1829,7 +1835,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -1849,7 +1855,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1873,7 +1879,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>64</v>
@@ -1900,7 +1906,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37"/>
       <c r="C16" s="19">
@@ -1925,7 +1931,7 @@
       <c r="J16" s="41"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37" t="s">
         <v>42</v>
@@ -1950,7 +1956,7 @@
       </c>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="37"/>
       <c r="C18" s="19"/>
@@ -1963,7 +1969,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:21" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>3</v>
       </c>
@@ -1980,7 +1986,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37" t="s">
         <v>66</v>
@@ -2006,7 +2012,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="37"/>
       <c r="C21" s="19">
@@ -2029,7 +2035,7 @@
       <c r="J21" s="41"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="37" t="s">
         <v>42</v>
@@ -2054,7 +2060,7 @@
       </c>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="37"/>
       <c r="C23" s="19"/>
@@ -2067,7 +2073,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>4</v>
       </c>
@@ -2084,7 +2090,7 @@
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="str">
         <f>B15</f>
@@ -2112,7 +2118,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37"/>
       <c r="C26" s="19">
@@ -2137,7 +2143,7 @@
       <c r="J26" s="41"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="37" t="s">
         <v>42</v>
@@ -2162,7 +2168,7 @@
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="37" t="s">
         <v>40</v>
@@ -2180,7 +2186,7 @@
       </c>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="37"/>
       <c r="C29" s="19"/>
@@ -2193,7 +2199,7 @@
       <c r="J29" s="41"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>5</v>
       </c>
@@ -2211,17 +2217,17 @@
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="87" t="s">
+      <c r="O30" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="87"/>
-      <c r="R30" s="87"/>
-      <c r="S30" s="87"/>
-      <c r="T30" s="87"/>
-      <c r="U30" s="87"/>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P30" s="84"/>
+      <c r="Q30" s="84"/>
+      <c r="R30" s="84"/>
+      <c r="S30" s="84"/>
+      <c r="T30" s="84"/>
+      <c r="U30" s="84"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37" t="str">
         <f>B36</f>
@@ -2257,7 +2263,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="37" t="s">
         <v>42</v>
@@ -2282,7 +2288,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>40</v>
@@ -2300,7 +2306,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37"/>
       <c r="C34" s="42"/>
@@ -2313,7 +2319,7 @@
       <c r="J34" s="45"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <v>6</v>
       </c>
@@ -2337,7 +2343,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="37" t="s">
         <v>62</v>
@@ -2372,7 +2378,7 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="37"/>
       <c r="C37" s="36">
@@ -2404,7 +2410,7 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="37" t="str">
         <f>B25</f>
@@ -2441,7 +2447,7 @@
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="37"/>
       <c r="C39" s="47">
@@ -2475,7 +2481,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="37" t="s">
         <v>73</v>
@@ -2509,7 +2515,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="37"/>
       <c r="C41" s="47">
@@ -2541,7 +2547,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="37" t="s">
         <v>42</v>
@@ -2566,7 +2572,7 @@
       </c>
       <c r="K42" s="36"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="37" t="s">
         <v>40</v>
@@ -2584,7 +2590,7 @@
       </c>
       <c r="K43" s="36"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="37"/>
       <c r="C44" s="42"/>
@@ -2597,7 +2603,7 @@
       <c r="J44" s="45"/>
       <c r="K44" s="36"/>
     </row>
-    <row r="45" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A45" s="63">
         <v>7</v>
       </c>
@@ -2614,7 +2620,7 @@
       <c r="J45" s="45"/>
       <c r="K45" s="29"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>62</v>
@@ -2649,7 +2655,7 @@
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="37" t="s">
         <v>42</v>
@@ -2674,7 +2680,7 @@
       </c>
       <c r="K47" s="36"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="37" t="s">
         <v>40</v>
@@ -2692,7 +2698,7 @@
       </c>
       <c r="K48" s="36"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="37"/>
       <c r="C49" s="42"/>
@@ -2705,7 +2711,7 @@
       <c r="J49" s="44"/>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
         <v>8</v>
       </c>
@@ -2722,7 +2728,7 @@
       <c r="J50" s="41"/>
       <c r="K50" s="21"/>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="B51" s="37" t="s">
         <v>56</v>
@@ -2748,7 +2754,7 @@
       <c r="J51" s="40"/>
       <c r="K51" s="21"/>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="37"/>
       <c r="C52" s="36">
@@ -2772,7 +2778,7 @@
       <c r="J52" s="40"/>
       <c r="K52" s="21"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="37" t="s">
         <v>59</v>
@@ -2798,7 +2804,7 @@
       <c r="J53" s="40"/>
       <c r="K53" s="21"/>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="37"/>
       <c r="C54" s="36">
@@ -2822,7 +2828,7 @@
       <c r="J54" s="40"/>
       <c r="K54" s="21"/>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
       <c r="B55" s="37" t="s">
         <v>60</v>
@@ -2848,7 +2854,7 @@
       <c r="J55" s="40"/>
       <c r="K55" s="21"/>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="B56" s="37" t="s">
         <v>76</v>
@@ -2868,7 +2874,7 @@
       <c r="J56" s="40"/>
       <c r="K56" s="21"/>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="37" t="s">
         <v>42</v>
@@ -2893,7 +2899,7 @@
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18"/>
       <c r="B58" s="37" t="s">
         <v>40</v>
@@ -2911,7 +2917,7 @@
       </c>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="37"/>
       <c r="C59" s="19"/>
@@ -2924,7 +2930,7 @@
       <c r="J59" s="41"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.3">
       <c r="A60" s="18">
         <v>9</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>37.665999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="37" t="str">
         <f>B38</f>
@@ -2986,7 +2992,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="37"/>
       <c r="C62" s="47">
@@ -3013,7 +3019,7 @@
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="37"/>
       <c r="C63" s="47">
@@ -3039,7 +3045,7 @@
       <c r="J63" s="40"/>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="37"/>
       <c r="C64" s="47">
@@ -3066,7 +3072,7 @@
       <c r="J64" s="40"/>
       <c r="K64" s="21"/>
     </row>
-    <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="37" t="s">
         <v>75</v>
@@ -3092,7 +3098,7 @@
       <c r="J65" s="40"/>
       <c r="K65" s="21"/>
     </row>
-    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="37" t="s">
         <v>42</v>
@@ -3117,7 +3123,7 @@
       </c>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
       <c r="B67" s="37" t="s">
         <v>40</v>
@@ -3139,7 +3145,7 @@
         <v>4.2669917708015843</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="37"/>
       <c r="C68" s="19"/>
@@ -3152,7 +3158,7 @@
       <c r="J68" s="41"/>
       <c r="K68" s="21"/>
     </row>
-    <row r="69" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A69" s="18">
         <v>10</v>
       </c>
@@ -3179,7 +3185,7 @@
       <c r="J69" s="41"/>
       <c r="K69" s="21"/>
     </row>
-    <row r="70" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="B70" s="37" t="s">
         <v>71</v>
@@ -3208,7 +3214,7 @@
       <c r="J70" s="41"/>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="37" t="s">
         <v>72</v>
@@ -3238,7 +3244,7 @@
       <c r="J71" s="41"/>
       <c r="K71" s="21"/>
     </row>
-    <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="37" t="s">
         <v>42</v>
@@ -3263,7 +3269,7 @@
       </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="37" t="s">
         <v>40</v>
@@ -3281,7 +3287,7 @@
       </c>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="37"/>
       <c r="C74" s="19"/>
@@ -3294,7 +3300,7 @@
       <c r="J74" s="41"/>
       <c r="K74" s="21"/>
     </row>
-    <row r="75" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>11</v>
       </c>
@@ -3311,7 +3317,7 @@
       <c r="J75" s="41"/>
       <c r="K75" s="21"/>
     </row>
-    <row r="76" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18"/>
       <c r="B76" s="37" t="s">
         <v>56</v>
@@ -3336,7 +3342,7 @@
       <c r="J76" s="40"/>
       <c r="K76" s="21"/>
     </row>
-    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18"/>
       <c r="B77" s="37"/>
       <c r="C77" s="36">
@@ -3359,7 +3365,7 @@
       <c r="J77" s="40"/>
       <c r="K77" s="21"/>
     </row>
-    <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="37" t="s">
         <v>42</v>
@@ -3384,7 +3390,7 @@
       </c>
       <c r="K78" s="21"/>
     </row>
-    <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="37" t="s">
         <v>40</v>
@@ -3402,7 +3408,7 @@
       </c>
       <c r="K79" s="21"/>
     </row>
-    <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
       <c r="B80" s="37"/>
       <c r="C80" s="19"/>
@@ -3415,7 +3421,7 @@
       <c r="J80" s="41"/>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>12</v>
       </c>
@@ -3451,7 +3457,7 @@
       <c r="R81" s="25"/>
       <c r="S81" s="25"/>
     </row>
-    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18"/>
       <c r="B82" s="24"/>
       <c r="C82" s="19"/>
@@ -3474,7 +3480,7 @@
       <c r="R82" s="25"/>
       <c r="S82" s="25"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="46" t="s">
         <v>17</v>
@@ -3492,7 +3498,7 @@
       </c>
       <c r="K83" s="36"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="58"/>
       <c r="B84" s="61"/>
       <c r="C84" s="62"/>
@@ -3505,16 +3511,16 @@
       <c r="J84" s="60"/>
       <c r="K84" s="57"/>
     </row>
-    <row r="85" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="50"/>
       <c r="B85" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C85" s="83">
+      <c r="C85" s="91">
         <f>J83</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D85" s="83"/>
+      <c r="D85" s="91"/>
       <c r="E85" s="39">
         <v>100</v>
       </c>
@@ -3525,15 +3531,15 @@
       <c r="J85" s="54"/>
       <c r="K85" s="55"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="56"/>
       <c r="B86" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="86">
+      <c r="C86" s="94">
         <v>500000</v>
       </c>
-      <c r="D86" s="86"/>
+      <c r="D86" s="94"/>
       <c r="E86" s="39"/>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -3542,16 +3548,16 @@
       <c r="J86" s="48"/>
       <c r="K86" s="49"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="56"/>
       <c r="B87" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="86">
+      <c r="C87" s="94">
         <f>C86-C89-C90</f>
         <v>475000</v>
       </c>
-      <c r="D87" s="86"/>
+      <c r="D87" s="94"/>
       <c r="E87" s="39">
         <f>C87/C85*100</f>
         <v>84.274408192973809</v>
@@ -3563,16 +3569,16 @@
       <c r="J87" s="48"/>
       <c r="K87" s="49"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="56"/>
       <c r="B88" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C88" s="83">
+      <c r="C88" s="91">
         <f>C85-C87</f>
         <v>88634.928070135182</v>
       </c>
-      <c r="D88" s="83"/>
+      <c r="D88" s="91"/>
       <c r="E88" s="39">
         <f>100-E87</f>
         <v>15.725591807026191</v>
@@ -3584,16 +3590,16 @@
       <c r="J88" s="48"/>
       <c r="K88" s="49"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="56"/>
       <c r="B89" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="83">
+      <c r="C89" s="91">
         <f>C86*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D89" s="83"/>
+      <c r="D89" s="91"/>
       <c r="E89" s="39">
         <v>3</v>
       </c>
@@ -3604,16 +3610,16 @@
       <c r="J89" s="48"/>
       <c r="K89" s="49"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="56"/>
       <c r="B90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="83">
+      <c r="C90" s="91">
         <f>C86*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D90" s="83"/>
+      <c r="D90" s="91"/>
       <c r="E90" s="39">
         <v>2</v>
       </c>
@@ -3624,7 +3630,7 @@
       <c r="J90" s="48"/>
       <c r="K90" s="49"/>
     </row>
-    <row r="91" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="57"/>
       <c r="B91" s="57"/>
       <c r="C91" s="57"/>
@@ -3637,64 +3643,72 @@
       <c r="J91" s="57"/>
       <c r="K91" s="57"/>
     </row>
-    <row r="92" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
     <mergeCell ref="O30:U30"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
@@ -3703,14 +3717,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -3723,115 +3729,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-    </row>
-    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="104" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+    </row>
+    <row r="2" spans="1:14" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="105" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+    </row>
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-    </row>
-    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+    </row>
+    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="101">
+      <c r="C6" s="95">
         <f>F46</f>
         <v>563634.92807013518</v>
       </c>
-      <c r="D6" s="102"/>
+      <c r="D6" s="96"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3839,90 +3845,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="101">
+      <c r="J6" s="95">
         <f>I46</f>
         <v>564688.31314685999</v>
       </c>
-      <c r="K6" s="102"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K6" s="96"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="I7" s="97" t="s">
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="I7" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="str">
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="85" t="str">
         <f>'Estimate (3)'!A6:F6</f>
         <v>Project:- गणपति ढिकुरेपाटी संरक्षण</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="I8" s="98" t="s">
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="I8" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="str">
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="105" t="str">
         <f>'Estimate (3)'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="I9" s="98" t="s">
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="I9" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100" t="s">
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="94" t="s">
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="95" t="s">
+      <c r="K11" s="101" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="100"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3941,10 +3947,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="94"/>
-      <c r="K12" s="95"/>
-    </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="100"/>
+      <c r="K12" s="101"/>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <f>'Estimate (3)'!A9</f>
         <v>1</v>
@@ -3995,7 +4001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="77" t="str">
         <f>'Estimate (3)'!B12</f>
@@ -4028,7 +4034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -4041,7 +4047,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>'Estimate (3)'!A14</f>
         <v>2</v>
@@ -4092,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -4108,7 +4114,7 @@
       </c>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <f>'Estimate (3)'!A19</f>
         <v>3</v>
@@ -4159,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="12"/>
@@ -4172,7 +4178,7 @@
       <c r="J19" s="28"/>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f>'Estimate (3)'!A24</f>
         <v>4</v>
@@ -4223,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="77" t="str">
         <f>'Estimate (3)'!B28</f>
@@ -4256,7 +4262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="12"/>
@@ -4269,7 +4275,7 @@
       <c r="J22" s="28"/>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <f>'Estimate (3)'!A30</f>
         <v>5</v>
@@ -4320,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="77" t="str">
         <f>'Estimate (3)'!B33</f>
@@ -4353,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="12"/>
@@ -4366,7 +4372,7 @@
       <c r="J25" s="28"/>
       <c r="K25" s="14"/>
     </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <f>'Estimate (3)'!A35</f>
         <v>6</v>
@@ -4417,7 +4423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
       <c r="B27" s="77" t="str">
         <f>'Estimate (3)'!B43</f>
@@ -4450,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="12"/>
@@ -4463,7 +4469,7 @@
       <c r="J28" s="28"/>
       <c r="K28" s="14"/>
     </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <f>'Estimate (3)'!A45</f>
         <v>7</v>
@@ -4514,7 +4520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="77" t="str">
         <f>'Estimate (3)'!B48</f>
@@ -4547,7 +4553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="12"/>
@@ -4560,7 +4566,7 @@
       <c r="J31" s="28"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <f>'Estimate (3)'!A50</f>
         <v>8</v>
@@ -4611,7 +4617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
       <c r="B33" s="77" t="str">
         <f>'Estimate (3)'!B58</f>
@@ -4644,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="12"/>
@@ -4657,7 +4663,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="14"/>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f>'Estimate (3)'!A60</f>
         <v>9</v>
@@ -4708,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
       <c r="B36" s="77" t="str">
         <f>'Estimate (3)'!B67</f>
@@ -4741,7 +4747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="12"/>
@@ -4754,7 +4760,7 @@
       <c r="J37" s="28"/>
       <c r="K37" s="14"/>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <f>'Estimate (3)'!A69</f>
         <v>10</v>
@@ -4805,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
       <c r="B39" s="77" t="str">
         <f>'Estimate (3)'!B73</f>
@@ -4838,7 +4844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="12"/>
@@ -4851,7 +4857,7 @@
       <c r="J40" s="28"/>
       <c r="K40" s="14"/>
     </row>
-    <row r="41" spans="1:14" s="76" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="72">
         <f>'Estimate (3)'!A75</f>
         <v>11</v>
@@ -4902,7 +4908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
       <c r="B42" s="77" t="str">
         <f>'Estimate (3)'!B79</f>
@@ -4935,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="12"/>
@@ -4948,7 +4954,7 @@
       <c r="J43" s="28"/>
       <c r="K43" s="14"/>
     </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <f>'Estimate (3)'!A81</f>
         <v>12</v>
@@ -4999,7 +5005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="12"/>
@@ -5012,7 +5018,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="14"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6" t="s">
         <v>16</v>
@@ -5037,38 +5043,38 @@
       <c r="K46" s="5"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="49" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="M49" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="N49" s="106" t="s">
+      <c r="N49" s="83" t="s">
         <v>87</v>
       </c>
       <c r="O49" s="78" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M50" s="78" t="s">
         <v>88</v>
       </c>
       <c r="N50" s="79">
-        <f>(1225/360*G13)+(612.5/10*G20)+(3675/5*G23)+(3675/15*G26)+(8575/5*G29)+(980/100*G32)</f>
-        <v>63199.748264034926</v>
+        <f>(1225/360*G13)+(612.5/10*G20)+(3675/5*G23)+(3675/15*G26)+(8575/5*G29)+(980/100*G32)+(1837.5*G35)+(14700*G38)+(14700/100*G41)</f>
+        <v>85610.002071868876</v>
       </c>
       <c r="O50" s="80"/>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M51" s="78" t="s">
         <v>89</v>
       </c>
       <c r="N51" s="79">
-        <f>(2760/360*G13)+(G16*H16)+(G18*H18)+(920/10*G20)+(3680/5*G23)+(27600/15*G26)+(12880/5*G29)+(644/100*G32)</f>
-        <v>98486.481054841817</v>
+        <f>(2760/360*G13)+(G16*H16)+(G18*H18)+(920/10*G20)+(3680/5*G23)+(27600/15*G26)+(12880/5*G29)+(644/100*G32)+((2024+184)*G35)+(11040*G38)+(14720/100*G41)</f>
+        <v>123290.83846851448</v>
       </c>
       <c r="O51" s="80"/>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M52" s="78" t="s">
         <v>85</v>
       </c>
@@ -5081,33 +5087,33 @@
         <v>144.73284800000005</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M53" s="78" t="s">
         <v>90</v>
       </c>
       <c r="N53" s="82">
-        <f>(6360.9/10*G20)</f>
-        <v>4288.8807948908861</v>
+        <f>(6360.9/10*G20)+(8481.2*G35)</f>
+        <v>65428.657792967024</v>
       </c>
       <c r="O53" s="81">
         <f t="shared" ref="O53:O54" si="2">N53*0.13</f>
-        <v>557.55450333581518</v>
-      </c>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+        <v>8505.7255130857138</v>
+      </c>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M54" s="78" t="s">
         <v>91</v>
       </c>
       <c r="N54" s="82">
-        <f>(2256.3/10*G20)+(21432.6/15*G26)+(6604.416/5*G29)</f>
-        <v>50887.772728778917</v>
+        <f>(2256.3/10*G20)+(21432.6/15*G26)+(6604.416/5*G29)+(953.37*G35)+(4639.73/100*G41)</f>
+        <v>60288.207767742817</v>
       </c>
       <c r="O54" s="81">
         <f t="shared" si="2"/>
-        <v>6615.4104547412589</v>
-      </c>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+        <v>7837.4670098065662</v>
+      </c>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M55" s="78" t="s">
         <v>92</v>
       </c>
@@ -5120,7 +5126,7 @@
         <v>14481.866457185406</v>
       </c>
     </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M56" s="78" t="s">
         <v>93</v>
       </c>
@@ -5133,33 +5139,33 @@
         <v>984.09317808449919</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M57" s="78" t="s">
         <v>94</v>
       </c>
       <c r="N57" s="82">
-        <f>(49275.03/15*G26)+(5368.95/5*G29)</f>
-        <v>45664.403091096428</v>
+        <f>(49275.03/15*G26)+(5368.95/5*G29)+(849.17*G35)+(6526.47/100*G41)</f>
+        <v>55341.570949107503</v>
       </c>
       <c r="O57" s="82">
         <f>0.13*N57</f>
-        <v>5936.3724018425355</v>
-      </c>
-    </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+        <v>7194.4042233839755</v>
+      </c>
+    </row>
+    <row r="58" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M58" s="78" t="s">
         <v>95</v>
       </c>
       <c r="N58" s="82">
-        <f>(620/15*G26)+(310/5*G29)</f>
-        <v>2250.1252934175404</v>
+        <f>(620/15*G26)+(310/5*G29)+(28*G35)</f>
+        <v>2451.9733521764579</v>
       </c>
       <c r="O58" s="82">
         <f>0.13*N58</f>
-        <v>292.51628814428028</v>
-      </c>
-    </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+        <v>318.75653578293952</v>
+      </c>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M59" s="78" t="s">
         <v>96</v>
       </c>
@@ -5172,7 +5178,7 @@
         <v>138.54427540905195</v>
       </c>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C60" s="82"/>
       <c r="D60" s="82"/>
       <c r="M60" s="78" t="s">
@@ -5182,8 +5188,12 @@
         <f>(350/100*G32)</f>
         <v>203.44664973704965</v>
       </c>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="82">
+        <f t="shared" ref="O60:O63" si="3">0.13*N60</f>
+        <v>26.448064465816454</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C61" s="82"/>
       <c r="D61" s="82"/>
       <c r="M61" s="78" t="s">
@@ -5193,148 +5203,191 @@
         <f>(108.4/100*G32)</f>
         <v>63.010333804274815</v>
       </c>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="82">
+        <f t="shared" si="3"/>
+        <v>8.1913433945557266</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C62" s="82"/>
       <c r="D62" s="82"/>
-    </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M62" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="N62">
+        <f>(105000*G38)</f>
+        <v>8252.9639412855904</v>
+      </c>
+      <c r="O62" s="82">
+        <f t="shared" si="3"/>
+        <v>1072.8853123671267</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C63" s="82"/>
       <c r="D63" s="82"/>
-    </row>
-    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M63" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="N63">
+        <f>(1200*G38)</f>
+        <v>94.319587900406759</v>
+      </c>
+      <c r="O63" s="82">
+        <f t="shared" si="3"/>
+        <v>12.261546427052879</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C64" s="82"/>
       <c r="D64" s="82"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C65" s="82"/>
       <c r="D65" s="82"/>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="N65" s="82">
+        <f>SUM(N50:N63)</f>
+        <v>522172.96598186577</v>
+      </c>
+      <c r="O65" s="82">
+        <f>SUM(O52:O63)</f>
+        <v>40725.376307392711</v>
+      </c>
+      <c r="P65" s="82">
+        <f>N65+O65-I46</f>
+        <v>-1789.9708576014964</v>
+      </c>
+    </row>
+    <row r="66" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C66" s="82"/>
       <c r="D66" s="82"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C67" s="82"/>
       <c r="D67" s="82"/>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="N67" s="82">
+        <f>N65-P65</f>
+        <v>523962.93683946726</v>
+      </c>
+      <c r="O67" s="82">
+        <f>O65</f>
+        <v>40725.376307392711</v>
+      </c>
+      <c r="P67" s="82">
+        <f>N67+O67-I46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C68" s="82"/>
       <c r="D68" s="82"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C69" s="82"/>
       <c r="D69" s="82"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C70" s="82"/>
       <c r="D70" s="82"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C71" s="82"/>
       <c r="D71" s="82"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C72" s="82"/>
       <c r="D72" s="82"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C73" s="82"/>
       <c r="D73" s="82"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C74" s="82"/>
       <c r="D74" s="82"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C75" s="82"/>
       <c r="D75" s="82"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C76" s="82"/>
       <c r="D76" s="82"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C77" s="82"/>
       <c r="D77" s="82"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C78" s="82"/>
       <c r="D78" s="82"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C79" s="82"/>
       <c r="D79" s="82"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C80" s="82"/>
       <c r="D80" s="82"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="82"/>
       <c r="D81" s="82"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="82"/>
       <c r="D82" s="82"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="82"/>
       <c r="D83" s="82"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="82"/>
       <c r="D84" s="82"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="82"/>
       <c r="D85" s="82"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="82"/>
       <c r="D86" s="82"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="82"/>
       <c r="D87" s="82"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="82"/>
       <c r="D88" s="82"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" s="82"/>
       <c r="D89" s="82"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" s="82"/>
       <c r="D90" s="82"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" s="82"/>
       <c r="D91" s="82"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" s="82"/>
       <c r="D92" s="82"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" s="82"/>
       <c r="D93" s="82"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" s="82"/>
       <c r="D94" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -5348,6 +5401,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5365,134 +5425,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="93" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+    </row>
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="88"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5527,7 +5587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="138" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -5544,7 +5604,7 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="37" t="str">
         <f>B30</f>
@@ -5574,7 +5634,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="37" t="s">
         <v>42</v>
@@ -5601,7 +5661,7 @@
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
         <v>40</v>
@@ -5621,7 +5681,7 @@
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37"/>
       <c r="C13" s="19"/>
@@ -5636,7 +5696,7 @@
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
     </row>
-    <row r="14" spans="1:14" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -5655,7 +5715,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="37" t="s">
         <v>64</v>
@@ -5682,7 +5742,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="37" t="s">
         <v>42</v>
@@ -5707,7 +5767,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="37"/>
       <c r="C17" s="19"/>
@@ -5720,7 +5780,7 @@
       <c r="J17" s="41"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:16" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -5737,7 +5797,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="37" t="s">
         <v>66</v>
@@ -5763,7 +5823,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="37"/>
       <c r="C20" s="19">
@@ -5786,7 +5846,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="37" t="s">
         <v>42</v>
@@ -5811,7 +5871,7 @@
       </c>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="37"/>
       <c r="C22" s="19"/>
@@ -5824,7 +5884,7 @@
       <c r="J22" s="41"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>4</v>
       </c>
@@ -5841,7 +5901,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="37" t="str">
         <f>B15</f>
@@ -5867,7 +5927,7 @@
       <c r="J24" s="41"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="37" t="s">
         <v>80</v>
@@ -5892,7 +5952,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="37" t="s">
         <v>42</v>
@@ -5917,7 +5977,7 @@
       </c>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="37" t="s">
         <v>40</v>
@@ -5935,7 +5995,7 @@
       </c>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="37"/>
       <c r="C28" s="19"/>
@@ -5948,7 +6008,7 @@
       <c r="J28" s="41"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>5</v>
       </c>
@@ -5964,12 +6024,12 @@
       <c r="I29" s="23"/>
       <c r="J29" s="41"/>
       <c r="K29" s="21"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
-    </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="84"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="37" t="str">
         <f>B37</f>
@@ -5999,7 +6059,7 @@
       <c r="M30" s="25"/>
       <c r="N30" s="25"/>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="37"/>
       <c r="C31" s="36">
@@ -6026,7 +6086,7 @@
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="37"/>
       <c r="C32" s="36">
@@ -6053,7 +6113,7 @@
       <c r="M32" s="25"/>
       <c r="N32" s="25"/>
     </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="37" t="s">
         <v>42</v>
@@ -6078,7 +6138,7 @@
       </c>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="37" t="s">
         <v>40</v>
@@ -6096,7 +6156,7 @@
       </c>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="37"/>
       <c r="C35" s="42"/>
@@ -6109,7 +6169,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="36"/>
     </row>
-    <row r="36" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="69" x14ac:dyDescent="0.3">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -6128,7 +6188,7 @@
       <c r="M36" s="25"/>
       <c r="N36" s="25"/>
     </row>
-    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="37" t="s">
         <v>62</v>
@@ -6157,7 +6217,7 @@
       <c r="M37" s="25"/>
       <c r="N37" s="25"/>
     </row>
-    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="37"/>
       <c r="C38" s="36">
@@ -6184,7 +6244,7 @@
       <c r="M38" s="25"/>
       <c r="N38" s="25"/>
     </row>
-    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="37" t="s">
         <v>62</v>
@@ -6213,7 +6273,7 @@
       <c r="M39" s="25"/>
       <c r="N39" s="25"/>
     </row>
-    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="37"/>
       <c r="C40" s="36">
@@ -6240,7 +6300,7 @@
       <c r="M40" s="25"/>
       <c r="N40" s="25"/>
     </row>
-    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="37" t="s">
         <v>62</v>
@@ -6269,7 +6329,7 @@
       <c r="M41" s="25"/>
       <c r="N41" s="25"/>
     </row>
-    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="37"/>
       <c r="C42" s="36">
@@ -6296,7 +6356,7 @@
       <c r="M42" s="25"/>
       <c r="N42" s="25"/>
     </row>
-    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="37" t="s">
         <v>73</v>
@@ -6326,7 +6386,7 @@
       <c r="M43" s="25"/>
       <c r="N43" s="25"/>
     </row>
-    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="37"/>
       <c r="C44" s="47">
@@ -6353,7 +6413,7 @@
       <c r="M44" s="25"/>
       <c r="N44" s="25"/>
     </row>
-    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18"/>
       <c r="B45" s="37"/>
       <c r="C45" s="47">
@@ -6380,7 +6440,7 @@
       <c r="M45" s="25"/>
       <c r="N45" s="25"/>
     </row>
-    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>80</v>
@@ -6410,7 +6470,7 @@
       <c r="M46" s="25"/>
       <c r="N46" s="25"/>
     </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="37"/>
       <c r="C47" s="47">
@@ -6437,7 +6497,7 @@
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
     </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="37" t="s">
         <v>42</v>
@@ -6462,7 +6522,7 @@
       </c>
       <c r="K48" s="36"/>
     </row>
-    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="37" t="s">
         <v>40</v>
@@ -6480,7 +6540,7 @@
       </c>
       <c r="K49" s="36"/>
     </row>
-    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="37"/>
       <c r="C50" s="42"/>
@@ -6493,7 +6553,7 @@
       <c r="J50" s="45"/>
       <c r="K50" s="36"/>
     </row>
-    <row r="51" spans="1:14" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A51" s="63">
         <v>7</v>
       </c>
@@ -6510,7 +6570,7 @@
       <c r="J51" s="45"/>
       <c r="K51" s="29"/>
     </row>
-    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="37" t="s">
         <v>62</v>
@@ -6540,7 +6600,7 @@
       <c r="M52" s="25"/>
       <c r="N52" s="25"/>
     </row>
-    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="37"/>
       <c r="C53" s="36">
@@ -6568,7 +6628,7 @@
       <c r="M53" s="25"/>
       <c r="N53" s="25"/>
     </row>
-    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="37"/>
       <c r="C54" s="36">
@@ -6596,7 +6656,7 @@
       <c r="M54" s="25"/>
       <c r="N54" s="25"/>
     </row>
-    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="37" t="s">
         <v>42</v>
@@ -6621,7 +6681,7 @@
       </c>
       <c r="K55" s="36"/>
     </row>
-    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="37" t="s">
         <v>40</v>
@@ -6639,7 +6699,7 @@
       </c>
       <c r="K56" s="36"/>
     </row>
-    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="37"/>
       <c r="C57" s="42"/>
@@ -6652,7 +6712,7 @@
       <c r="J57" s="44"/>
       <c r="K57" s="36"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
         <v>8</v>
       </c>
@@ -6669,7 +6729,7 @@
       <c r="J58" s="41"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="37" t="s">
         <v>56</v>
@@ -6695,7 +6755,7 @@
       <c r="J59" s="40"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="37" t="s">
         <v>59</v>
@@ -6721,7 +6781,7 @@
       <c r="J60" s="40"/>
       <c r="K60" s="21"/>
     </row>
-    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="37"/>
       <c r="C61" s="36">
@@ -6745,7 +6805,7 @@
       <c r="J61" s="40"/>
       <c r="K61" s="21"/>
     </row>
-    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="37" t="s">
         <v>60</v>
@@ -6771,7 +6831,7 @@
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="37" t="s">
         <v>42</v>
@@ -6796,7 +6856,7 @@
       </c>
       <c r="K63" s="21"/>
     </row>
-    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="37" t="s">
         <v>40</v>
@@ -6814,7 +6874,7 @@
       </c>
       <c r="K64" s="21"/>
     </row>
-    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="37"/>
       <c r="C65" s="19"/>
@@ -6827,7 +6887,7 @@
       <c r="J65" s="41"/>
       <c r="K65" s="21"/>
     </row>
-    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A66" s="18">
         <v>9</v>
       </c>
@@ -6844,7 +6904,7 @@
       <c r="J66" s="41"/>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18"/>
       <c r="B67" s="37" t="s">
         <v>56</v>
@@ -6872,7 +6932,7 @@
       <c r="J67" s="40"/>
       <c r="K67" s="21"/>
     </row>
-    <row r="68" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="37"/>
       <c r="C68" s="47">
@@ -6897,7 +6957,7 @@
       <c r="J68" s="40"/>
       <c r="K68" s="21"/>
     </row>
-    <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="37" t="s">
         <v>79</v>
@@ -6924,7 +6984,7 @@
       <c r="J69" s="40"/>
       <c r="K69" s="21"/>
     </row>
-    <row r="70" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="B70" s="37" t="s">
         <v>78</v>
@@ -6953,7 +7013,7 @@
       <c r="J70" s="40"/>
       <c r="K70" s="21"/>
     </row>
-    <row r="71" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="37" t="s">
         <v>81</v>
@@ -6979,7 +7039,7 @@
       <c r="J71" s="40"/>
       <c r="K71" s="21"/>
     </row>
-    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="37" t="s">
         <v>42</v>
@@ -7004,7 +7064,7 @@
       </c>
       <c r="K72" s="21"/>
     </row>
-    <row r="73" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="37" t="s">
         <v>40</v>
@@ -7022,7 +7082,7 @@
       </c>
       <c r="K73" s="21"/>
     </row>
-    <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="37"/>
       <c r="C74" s="19"/>
@@ -7035,7 +7095,7 @@
       <c r="J74" s="41"/>
       <c r="K74" s="21"/>
     </row>
-    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>10</v>
       </c>
@@ -7062,7 +7122,7 @@
       <c r="J75" s="41"/>
       <c r="K75" s="21"/>
     </row>
-    <row r="76" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18"/>
       <c r="B76" s="37" t="s">
         <v>71</v>
@@ -7091,7 +7151,7 @@
       <c r="J76" s="41"/>
       <c r="K76" s="21"/>
     </row>
-    <row r="77" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18"/>
       <c r="B77" s="37" t="s">
         <v>72</v>
@@ -7121,7 +7181,7 @@
       <c r="J77" s="41"/>
       <c r="K77" s="21"/>
     </row>
-    <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="37" t="s">
         <v>42</v>
@@ -7146,7 +7206,7 @@
       </c>
       <c r="K78" s="21"/>
     </row>
-    <row r="79" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="37" t="s">
         <v>40</v>
@@ -7164,7 +7224,7 @@
       </c>
       <c r="K79" s="21"/>
     </row>
-    <row r="80" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18"/>
       <c r="B80" s="37"/>
       <c r="C80" s="19"/>
@@ -7177,7 +7237,7 @@
       <c r="J80" s="41"/>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:14" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>11</v>
       </c>
@@ -7194,7 +7254,7 @@
       <c r="J81" s="41"/>
       <c r="K81" s="21"/>
     </row>
-    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18"/>
       <c r="B82" s="37" t="s">
         <v>56</v>
@@ -7219,7 +7279,7 @@
       <c r="J82" s="40"/>
       <c r="K82" s="21"/>
     </row>
-    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="18"/>
       <c r="B83" s="37"/>
       <c r="C83" s="36">
@@ -7242,7 +7302,7 @@
       <c r="J83" s="40"/>
       <c r="K83" s="21"/>
     </row>
-    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="18"/>
       <c r="B84" s="37" t="s">
         <v>81</v>
@@ -7268,7 +7328,7 @@
       <c r="J84" s="40"/>
       <c r="K84" s="21"/>
     </row>
-    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18"/>
       <c r="B85" s="37" t="s">
         <v>42</v>
@@ -7293,7 +7353,7 @@
       </c>
       <c r="K85" s="21"/>
     </row>
-    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18"/>
       <c r="B86" s="37" t="s">
         <v>40</v>
@@ -7311,7 +7371,7 @@
       </c>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18"/>
       <c r="B87" s="37"/>
       <c r="C87" s="19"/>
@@ -7324,7 +7384,7 @@
       <c r="J87" s="41"/>
       <c r="K87" s="21"/>
     </row>
-    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="18">
         <v>12</v>
       </c>
@@ -7355,7 +7415,7 @@
       <c r="M88" s="25"/>
       <c r="N88" s="25"/>
     </row>
-    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="18"/>
       <c r="B89" s="24"/>
       <c r="C89" s="19"/>
@@ -7370,7 +7430,7 @@
       <c r="M89" s="25"/>
       <c r="N89" s="25"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="46" t="s">
         <v>17</v>
@@ -7388,7 +7448,7 @@
       </c>
       <c r="K90" s="36"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="58"/>
       <c r="B91" s="61"/>
       <c r="C91" s="62"/>
@@ -7401,16 +7461,16 @@
       <c r="J91" s="60"/>
       <c r="K91" s="57"/>
     </row>
-    <row r="92" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="50"/>
       <c r="B92" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="83">
+      <c r="C92" s="91">
         <f>J90</f>
         <v>564688.31314685999</v>
       </c>
-      <c r="D92" s="83"/>
+      <c r="D92" s="91"/>
       <c r="E92" s="39">
         <v>100</v>
       </c>
@@ -7421,15 +7481,15 @@
       <c r="J92" s="54"/>
       <c r="K92" s="55"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="56"/>
       <c r="B93" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C93" s="86">
+      <c r="C93" s="94">
         <v>500000</v>
       </c>
-      <c r="D93" s="86"/>
+      <c r="D93" s="94"/>
       <c r="E93" s="39"/>
       <c r="F93" s="49"/>
       <c r="G93" s="48"/>
@@ -7438,16 +7498,16 @@
       <c r="J93" s="48"/>
       <c r="K93" s="49"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="56"/>
       <c r="B94" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C94" s="86">
+      <c r="C94" s="94">
         <f>C93-C96-C97</f>
         <v>475000</v>
       </c>
-      <c r="D94" s="86"/>
+      <c r="D94" s="94"/>
       <c r="E94" s="39">
         <f>C94/C92*100</f>
         <v>84.117200399092638</v>
@@ -7459,16 +7519,16 @@
       <c r="J94" s="48"/>
       <c r="K94" s="49"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="56"/>
       <c r="B95" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C95" s="83">
+      <c r="C95" s="91">
         <f>C92-C94</f>
         <v>89688.31314685999</v>
       </c>
-      <c r="D95" s="83"/>
+      <c r="D95" s="91"/>
       <c r="E95" s="39">
         <f>100-E94</f>
         <v>15.882799600907362</v>
@@ -7480,16 +7540,16 @@
       <c r="J95" s="48"/>
       <c r="K95" s="49"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="56"/>
       <c r="B96" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C96" s="83">
+      <c r="C96" s="91">
         <f>C93*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D96" s="83"/>
+      <c r="D96" s="91"/>
       <c r="E96" s="39">
         <v>3</v>
       </c>
@@ -7500,16 +7560,16 @@
       <c r="J96" s="48"/>
       <c r="K96" s="49"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="56"/>
       <c r="B97" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C97" s="83">
+      <c r="C97" s="91">
         <f>C93*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D97" s="83"/>
+      <c r="D97" s="91"/>
       <c r="E97" s="39">
         <v>2</v>
       </c>
@@ -7520,7 +7580,7 @@
       <c r="J97" s="48"/>
       <c r="K97" s="49"/>
     </row>
-    <row r="98" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="57"/>
       <c r="B98" s="57"/>
       <c r="C98" s="57"/>
@@ -7533,64 +7593,69 @@
       <c r="J98" s="57"/>
       <c r="K98" s="57"/>
     </row>
-    <row r="99" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
     <mergeCell ref="M29:P29"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="C93:D93"/>
@@ -7602,11 +7667,6 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>